<commit_message>
added 2 bit adder and 4-bit counter
working on 4-bit adder
</commit_message>
<xml_diff>
--- a/CPU in Excel MAIN.xlsx
+++ b/CPU in Excel MAIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\100146766\Documents\CPU in Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BE346AB-7570-45EC-ACF7-33B5D8CB57CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D96ECC-59FC-4693-BC77-DF58103B6D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1B66EC66-FDED-4F04-B5B9-1656D0B4CE5B}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="30">
   <si>
     <t>CLOCK</t>
   </si>
@@ -130,6 +130,39 @@
   <si>
     <t>REVERSE DOWN COUNTER BITS TO MAKE UP COUNTER</t>
   </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>CARRY</t>
+  </si>
+  <si>
+    <t>BITA</t>
+  </si>
+  <si>
+    <t>BITB</t>
+  </si>
+  <si>
+    <t>2-BIT ADDER</t>
+  </si>
+  <si>
+    <t>OUT 4-BIT</t>
+  </si>
+  <si>
+    <t>SUB/ADD</t>
+  </si>
+  <si>
+    <t>INDEX 2</t>
+  </si>
+  <si>
+    <t>INDEX 1</t>
+  </si>
+  <si>
+    <t>INDEX 3</t>
+  </si>
+  <si>
+    <t>INDEX 4</t>
+  </si>
 </sst>
 </file>
 
@@ -164,7 +197,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -452,11 +485,131 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF339933"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF339933"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF339933"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF339933"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF339933"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF339933"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF339933"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF339933"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF339933"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF339933"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF339933"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF339933"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF339933"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF339933"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -489,15 +642,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
@@ -506,6 +650,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -518,12 +663,1005 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
+  <dxfs count="152">
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1399,10 +2537,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FC4233A-7F14-4F83-A44E-FF3D0836BCB8}">
-  <dimension ref="A1:Q21"/>
+  <dimension ref="A1:AG68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="T40" sqref="T40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1455,18 +2593,18 @@
       <c r="A4" s="2"/>
       <c r="G4" s="12"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="27"/>
+      <c r="I4" s="24"/>
       <c r="J4" s="3">
         <f ca="1">IF(CLOCK = 0, J4, IF(AND(CLOCK = 1,INPUT = 1,RESET = 0), 0, IF(AND(CLOCK = 1,INPUT = 0,RESET = 1), 1, IF(AND(CLOCK = 1,INPUT = 0,RESET = 0), J4, IF(AND(CLOCK = 1,INPUT = 1,RESET = 1),IF(JK.1 = 1, 0, 1))))))</f>
         <v>0</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="29"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="26"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -1478,37 +2616,37 @@
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="14"/>
-      <c r="I5" s="24"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="5">
         <f ca="1">IF(CLOCK = 0, J5, IF(AND(CLOCK = 1,JK.1 = 1,JK.1 = 0), 0, IF(AND(CLOCK = 1,JK.1 = 0,JK.1 = 1), 1, IF(AND(CLOCK = 1,JK.1 = 0, JK.1 = 0), J5, IF(AND(CLOCK = 1,JK.1 = 1,JK.1 = 1), IF(JK.2 = 1, 0, 1))))))</f>
         <v>0</v>
       </c>
-      <c r="K5" s="24"/>
+      <c r="K5" s="21"/>
       <c r="L5" s="18"/>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="33" t="s">
         <v>17</v>
       </c>
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
       <c r="P5" s="18"/>
-      <c r="Q5" s="30"/>
+      <c r="Q5" s="27"/>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="G6" s="13"/>
       <c r="H6" s="14"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="5">
         <f ca="1">IF(AND(JK.1 = 1, JK.2 = 1), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="L6" s="18"/>
-      <c r="M6" s="21"/>
+      <c r="M6" s="34"/>
       <c r="N6" s="18"/>
       <c r="O6" s="18"/>
       <c r="P6" s="18"/>
-      <c r="Q6" s="30"/>
+      <c r="Q6" s="27"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1519,26 +2657,26 @@
         <v>2</v>
       </c>
       <c r="G7" s="11"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="24"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="21"/>
       <c r="J7" s="5">
         <f ca="1">IF(CLOCK = 0, J7, IF(AND(CLOCK = 1,AND.1 = 1,AND.1 = 0), 0, IF(AND(CLOCK = 1,AND.1 = 0,AND.1 = 1), 1, IF(AND(CLOCK = 1,AND.1 = 0,AND.1 = 0), J7, IF(AND(CLOCK = 1,AND.1 = 1,AND.1 = 1), IF(JK.3 = 1, 0, 1))))))</f>
         <v>0</v>
       </c>
-      <c r="K7" s="24"/>
+      <c r="K7" s="21"/>
       <c r="L7" s="18"/>
-      <c r="M7" s="22"/>
+      <c r="M7" s="35"/>
       <c r="N7" s="18"/>
       <c r="O7" s="18"/>
       <c r="P7" s="18"/>
-      <c r="Q7" s="30"/>
+      <c r="Q7" s="27"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="G8" s="15"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="24"/>
-      <c r="J8" s="24"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
       <c r="K8" s="5" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">IF(AND(AND.1 = 1, JK.3 = 1), 1, 0)</f>
         <v>0</v>
@@ -1548,7 +2686,7 @@
       <c r="N8" s="18"/>
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
-      <c r="Q8" s="30"/>
+      <c r="Q8" s="27"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
@@ -1560,32 +2698,32 @@
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="24"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="5">
         <f ca="1">IF(CLOCK = 0, J9, IF(AND(CLOCK = 1,AND.2 = 1,AND.2 = 0), 0, IF(AND(CLOCK = 1,AND.2 = 0,AND.2 = 1), 1, IF(AND(CLOCK = 1,AND.2 = 0,AND.2 = 0), J9, IF(AND(CLOCK = 1,AND.2 = 1,AND.2 = 1), IF(JK.4 = 1, 0, 1))))))</f>
         <v>0</v>
       </c>
-      <c r="K9" s="24"/>
+      <c r="K9" s="21"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
       <c r="O9" s="18"/>
       <c r="P9" s="18"/>
-      <c r="Q9" s="30"/>
+      <c r="Q9" s="27"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="G10" s="13"/>
       <c r="H10" s="17"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
       <c r="O10" s="18"/>
       <c r="P10" s="18"/>
-      <c r="Q10" s="30"/>
+      <c r="Q10" s="27"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
@@ -1600,12 +2738,12 @@
       <c r="I11" s="10"/>
       <c r="J11" s="19"/>
       <c r="K11" s="19"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="O11" s="25"/>
-      <c r="P11" s="25"/>
-      <c r="Q11" s="35"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="28"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
@@ -1613,35 +2751,35 @@
         <f ca="1">IF(JK.4 = 1, 0, 1)</f>
         <v>1</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="21" t="s">
         <v>1</v>
       </c>
       <c r="I12" s="5">
         <f ca="1">IF(JK.3 = 1, 0, 1)</f>
         <v>1</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="21" t="s">
         <v>1</v>
       </c>
       <c r="K12" s="5">
         <f ca="1">IF(JK.2 = 1, 0, 1)</f>
         <v>1</v>
       </c>
-      <c r="L12" s="24" t="s">
+      <c r="L12" s="21" t="s">
         <v>1</v>
       </c>
       <c r="M12" s="5">
         <f ca="1">IF(JK.1 = 1, 0, 1)</f>
         <v>1</v>
       </c>
-      <c r="N12" s="24" t="s">
+      <c r="N12" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="O12" s="31" t="s">
+      <c r="O12" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="P12" s="31"/>
-      <c r="Q12" s="32"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="30"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -1659,9 +2797,9 @@
       <c r="L13" s="19"/>
       <c r="M13" s="19"/>
       <c r="N13" s="10"/>
-      <c r="O13" s="31"/>
-      <c r="P13" s="31"/>
-      <c r="Q13" s="32"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="30"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
@@ -1669,33 +2807,33 @@
         <f ca="1">NOT.4</f>
         <v>1</v>
       </c>
-      <c r="H14" s="26" t="s">
+      <c r="H14" s="23" t="s">
         <v>15</v>
       </c>
       <c r="I14" s="8">
         <f ca="1">NOT.3</f>
         <v>1</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="23" t="s">
         <v>14</v>
       </c>
       <c r="K14" s="8">
         <f ca="1">NOT.2</f>
         <v>1</v>
       </c>
-      <c r="L14" s="26" t="s">
+      <c r="L14" s="23" t="s">
         <v>13</v>
       </c>
       <c r="M14" s="8">
         <f ca="1">NOT.1</f>
         <v>1</v>
       </c>
-      <c r="N14" s="26" t="s">
+      <c r="N14" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="34"/>
+      <c r="O14" s="31"/>
+      <c r="P14" s="31"/>
+      <c r="Q14" s="32"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1709,7 +2847,7 @@
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f ca="1">IF(OR(AND(A3 = 1, C3 = 1), AND(A3 = 0, C3 = 0)), 1, 0)</f>
         <v>0</v>
@@ -1717,8 +2855,42 @@
       <c r="B17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="3">
+        <v>1</v>
+      </c>
+      <c r="L17" s="41" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" s="44"/>
+      <c r="N17" s="26"/>
+    </row>
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="5">
+        <v>1</v>
+      </c>
+      <c r="I18" s="5">
+        <v>0</v>
+      </c>
+      <c r="J18" s="5">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5">
+        <v>0</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M18" s="17"/>
+      <c r="N18" s="27"/>
+    </row>
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f ca="1">IF(AND(A1 = 1, C1 = 1), 0, IF(AND(A1 = 1, C1 = 0), 1, IF(AND(A1 = 0, C1 = 1), 0, A19)))</f>
         <v>1</v>
@@ -1726,8 +2898,38 @@
       <c r="B19" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="5">
+        <v>1</v>
+      </c>
+      <c r="I19" s="5">
+        <v>0</v>
+      </c>
+      <c r="J19" s="5">
+        <v>0</v>
+      </c>
+      <c r="K19" s="5">
+        <v>0</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="17"/>
+      <c r="N19" s="27"/>
+    </row>
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+      <c r="J20" s="17"/>
+      <c r="K20" s="17"/>
+      <c r="L20" s="17"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="27"/>
+    </row>
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f ca="1">IF(A1 = 0, A21, IF(AND(A1 = 1, C1 = 1, E1 = 0), 1, IF(AND(A1 = 1, C1 = 0, E1 = 1), 0, IF(AND(A1 = 1, C1 = 0, E1 = 0), A21, IF(AND(A1 = 1, C1 = 1, E1 = 1), IF(A21 = 1, 0, 1))))))</f>
         <v>1</v>
@@ -1735,157 +2937,1260 @@
       <c r="B21" t="s">
         <v>16</v>
       </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="17"/>
+      <c r="K21" s="17"/>
+      <c r="L21" s="17"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="27"/>
+    </row>
+    <row r="22" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="5">
+        <f>IF(_xlfn.XOR(K17 = 1, K19 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="27"/>
+    </row>
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F23" s="16"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="25"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="27"/>
+    </row>
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F24" s="16"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="5">
+        <v>0</v>
+      </c>
+      <c r="I24" s="5">
+        <f>K18</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="5">
+        <f>J22</f>
+        <v>1</v>
+      </c>
+      <c r="K24" s="18"/>
+      <c r="L24" s="27"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="27"/>
+    </row>
+    <row r="25" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F25" s="16"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="M25" s="17"/>
+      <c r="N25" s="27"/>
+      <c r="AG25" s="2"/>
+    </row>
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F26" s="16"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="5">
+        <f>IF(_xlfn.XOR(I24 = 1, J24 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K26" s="18"/>
+      <c r="L26" s="47"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F27" s="16"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="5">
+        <f>IF(AND(I24 = 1, J24 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="5">
+        <f>IF(AND(H24 = 1, J26 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J27" s="21"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="48"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="27"/>
+    </row>
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F28" s="16"/>
+      <c r="G28" s="13"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="5">
+        <f>IF(_xlfn.XOR(H24 = 1, J26 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K28" s="18"/>
+      <c r="L28" s="27"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="27"/>
+    </row>
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F29" s="16"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="5">
+        <f>IF(OR(H27 = 1, I27 =1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J29" s="21"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="27"/>
+    </row>
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F30" s="16"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="27"/>
+    </row>
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F31" s="16"/>
+      <c r="G31" s="36"/>
+      <c r="H31" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="8">
+        <f>I29</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="8">
+        <f>J28</f>
+        <v>1</v>
+      </c>
+      <c r="K31" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L31" s="37"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="27"/>
+    </row>
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="5">
+        <f>IF(_xlfn.XOR(K17 = 1, J19 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K32" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="27"/>
+    </row>
+    <row r="33" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F33" s="16"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I33" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J33" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K33" s="25"/>
+      <c r="L33" s="26"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="27"/>
+    </row>
+    <row r="34" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F34" s="16"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="5">
+        <f>I31</f>
+        <v>0</v>
+      </c>
+      <c r="I34" s="5">
+        <f>J18</f>
+        <v>0</v>
+      </c>
+      <c r="J34" s="5">
+        <f>J32</f>
+        <v>1</v>
+      </c>
+      <c r="K34" s="18"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="27"/>
+    </row>
+    <row r="35" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F35" s="16"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="M35" s="17"/>
+      <c r="N35" s="27"/>
+    </row>
+    <row r="36" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F36" s="16"/>
+      <c r="G36" s="13"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="5">
+        <f>IF(_xlfn.XOR(I34 = 1, J34 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K36" s="18"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="17"/>
+      <c r="N36" s="42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F37" s="16"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="5">
+        <f>IF(AND(I34 = 1, J34 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <f>IF(AND(H34 = 1, J36 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J37" s="21"/>
+      <c r="K37" s="18"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="27"/>
+    </row>
+    <row r="38" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F38" s="16"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="5">
+        <f>IF(_xlfn.XOR(H34 = 1, J36 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K38" s="18"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="27"/>
+    </row>
+    <row r="39" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F39" s="16"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="5">
+        <f>IF(OR(H37 = 1, I37 =1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J39" s="21"/>
+      <c r="K39" s="18"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="27"/>
+    </row>
+    <row r="40" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F40" s="16"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="18"/>
+      <c r="I40" s="18"/>
+      <c r="J40" s="18"/>
+      <c r="K40" s="18"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="17"/>
+      <c r="N40" s="27"/>
+    </row>
+    <row r="41" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F41" s="16"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="8">
+        <f>I39</f>
+        <v>0</v>
+      </c>
+      <c r="J41" s="8">
+        <f>J38</f>
+        <v>1</v>
+      </c>
+      <c r="K41" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L41" s="37"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="27"/>
+    </row>
+    <row r="42" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F42" s="16"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="5">
+        <f>IF(_xlfn.XOR(K17 = 1, I19 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L42" s="17"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="27"/>
+    </row>
+    <row r="43" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F43" s="16"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I43" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J43" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K43" s="25"/>
+      <c r="L43" s="26"/>
+      <c r="M43" s="17"/>
+      <c r="N43" s="27"/>
+    </row>
+    <row r="44" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F44" s="16"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="5">
+        <f>I41</f>
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <f>I18</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="5">
+        <v>0</v>
+      </c>
+      <c r="K44" s="18"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="27"/>
+    </row>
+    <row r="45" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F45" s="16"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="18"/>
+      <c r="I45" s="18"/>
+      <c r="J45" s="18"/>
+      <c r="K45" s="18"/>
+      <c r="L45" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="M45" s="17"/>
+      <c r="N45" s="27"/>
+    </row>
+    <row r="46" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F46" s="16"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="5">
+        <f>IF(_xlfn.XOR(I44 = 1, J44 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K46" s="18"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="42" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F47" s="16"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="5">
+        <f>IF(AND(I44 = 1, J44 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I47" s="5">
+        <f>IF(AND(H44 = 1, J46 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J47" s="21"/>
+      <c r="K47" s="18"/>
+      <c r="L47" s="40"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="27"/>
+    </row>
+    <row r="48" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F48" s="16"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="5">
+        <f>IF(_xlfn.XOR(H44 = 1, J46 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K48" s="18"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="27"/>
+    </row>
+    <row r="49" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F49" s="16"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="5">
+        <f>IF(OR(H47 = 1, I47 =1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J49" s="21"/>
+      <c r="K49" s="18"/>
+      <c r="L49" s="27"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="27"/>
+    </row>
+    <row r="50" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F50" s="16"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="18"/>
+      <c r="J50" s="18"/>
+      <c r="K50" s="18"/>
+      <c r="L50" s="27"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="27"/>
+    </row>
+    <row r="51" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F51" s="16"/>
+      <c r="G51" s="36"/>
+      <c r="H51" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I51" s="8">
+        <f>I49</f>
+        <v>0</v>
+      </c>
+      <c r="J51" s="8">
+        <f>J48</f>
+        <v>0</v>
+      </c>
+      <c r="K51" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L51" s="37"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="27"/>
+    </row>
+    <row r="52" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F52" s="16"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="5">
+        <f>IF(_xlfn.XOR(K17 = 1, H19 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="K52" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L52" s="17"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="27"/>
+    </row>
+    <row r="53" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F53" s="16"/>
+      <c r="G53" s="12"/>
+      <c r="H53" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I53" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="J53" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="K53" s="25"/>
+      <c r="L53" s="26"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="27"/>
+    </row>
+    <row r="54" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F54" s="16"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="5">
+        <f>I51</f>
+        <v>0</v>
+      </c>
+      <c r="I54" s="5">
+        <f>H18</f>
+        <v>1</v>
+      </c>
+      <c r="J54" s="5">
+        <v>0</v>
+      </c>
+      <c r="K54" s="18"/>
+      <c r="L54" s="27"/>
+      <c r="M54" s="17"/>
+      <c r="N54" s="27"/>
+    </row>
+    <row r="55" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F55" s="16"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="18"/>
+      <c r="I55" s="18"/>
+      <c r="J55" s="18"/>
+      <c r="K55" s="18"/>
+      <c r="L55" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="M55" s="17"/>
+      <c r="N55" s="27"/>
+    </row>
+    <row r="56" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F56" s="16"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
+      <c r="J56" s="5">
+        <f>IF(_xlfn.XOR(I54 = 1, J54 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K56" s="18"/>
+      <c r="L56" s="39"/>
+      <c r="M56" s="17"/>
+      <c r="N56" s="42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="57" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F57" s="16"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="5">
+        <f>IF(AND(I54 = 1, J54 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="I57" s="5">
+        <f>IF(AND(H54 = 1, J56 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J57" s="21"/>
+      <c r="K57" s="18"/>
+      <c r="L57" s="40"/>
+      <c r="M57" s="17"/>
+      <c r="N57" s="27"/>
+    </row>
+    <row r="58" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F58" s="16"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="5">
+        <f>IF(_xlfn.XOR(H54 = 1, J56 = 1), 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="K58" s="18"/>
+      <c r="L58" s="27"/>
+      <c r="M58" s="17"/>
+      <c r="N58" s="27"/>
+    </row>
+    <row r="59" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F59" s="16"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="5">
+        <f>IF(OR(H57 = 1, I57 =1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="J59" s="21"/>
+      <c r="K59" s="18"/>
+      <c r="L59" s="27"/>
+      <c r="M59" s="17"/>
+      <c r="N59" s="27"/>
+    </row>
+    <row r="60" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F60" s="16"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="18"/>
+      <c r="J60" s="18"/>
+      <c r="K60" s="18"/>
+      <c r="L60" s="27"/>
+      <c r="M60" s="17"/>
+      <c r="N60" s="27"/>
+    </row>
+    <row r="61" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F61" s="16"/>
+      <c r="G61" s="36"/>
+      <c r="H61" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="I61" s="8">
+        <f>I59</f>
+        <v>0</v>
+      </c>
+      <c r="J61" s="8">
+        <f>J58</f>
+        <v>1</v>
+      </c>
+      <c r="K61" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="L61" s="37"/>
+      <c r="M61" s="17"/>
+      <c r="N61" s="27"/>
+    </row>
+    <row r="62" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F62" s="16"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="17"/>
+      <c r="M62" s="17"/>
+      <c r="N62" s="27"/>
+    </row>
+    <row r="63" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F63" s="16"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+      <c r="J63" s="17"/>
+      <c r="K63" s="17"/>
+      <c r="L63" s="17"/>
+      <c r="M63" s="17"/>
+      <c r="N63" s="27"/>
+    </row>
+    <row r="64" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F64" s="16"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+      <c r="J64" s="17"/>
+      <c r="K64" s="17"/>
+      <c r="L64" s="17"/>
+      <c r="M64" s="17"/>
+      <c r="N64" s="27"/>
+    </row>
+    <row r="65" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F65" s="16"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+      <c r="J65" s="17"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17"/>
+      <c r="M65" s="17"/>
+      <c r="N65" s="27"/>
+    </row>
+    <row r="66" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F66" s="16"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+      <c r="J66" s="17"/>
+      <c r="K66" s="17"/>
+      <c r="L66" s="17"/>
+      <c r="M66" s="17"/>
+      <c r="N66" s="27"/>
+    </row>
+    <row r="67" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F67" s="16"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+      <c r="J67" s="17"/>
+      <c r="K67" s="17"/>
+      <c r="L67" s="17"/>
+      <c r="M67" s="17"/>
+      <c r="N67" s="27"/>
+    </row>
+    <row r="68" spans="6:14" x14ac:dyDescent="0.25">
+      <c r="F68" s="7">
+        <f>I61</f>
+        <v>0</v>
+      </c>
+      <c r="G68" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" s="8">
+        <f>J61</f>
+        <v>1</v>
+      </c>
+      <c r="I68" s="8">
+        <f>J51</f>
+        <v>0</v>
+      </c>
+      <c r="J68" s="8">
+        <f>J41</f>
+        <v>1</v>
+      </c>
+      <c r="K68" s="8">
+        <f>J31</f>
+        <v>1</v>
+      </c>
+      <c r="L68" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M68" s="45"/>
+      <c r="N68" s="37"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="L55:L57"/>
+    <mergeCell ref="L45:L47"/>
+    <mergeCell ref="L35:L37"/>
+    <mergeCell ref="L25:L27"/>
     <mergeCell ref="O12:Q14"/>
     <mergeCell ref="M5:M7"/>
   </mergeCells>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="55" priority="121" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="122" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="209" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="210" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="cellIs" dxfId="53" priority="99" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="100" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="187" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="148" priority="188" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="51" priority="97" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="98" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="185" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="146" priority="186" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="49" priority="95" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="96" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="183" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="184" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="47" priority="93" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="94" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="181" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="142" priority="182" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="45" priority="91" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="92" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="179" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="140" priority="180" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11">
-    <cfRule type="cellIs" dxfId="43" priority="89" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="177" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="178" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="41" priority="87" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="175" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="136" priority="176" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="39" priority="85" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="86" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="173" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="134" priority="174" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="37" priority="83" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="171" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="172" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="35" priority="73" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="74" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="161" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="130" priority="162" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="cellIs" dxfId="33" priority="71" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="159" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="128" priority="160" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="31" priority="53" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="141" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="142" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="29" priority="65" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="153" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="124" priority="154" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="27" priority="61" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="149" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="122" priority="150" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="25" priority="59" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="147" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="148" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="23" priority="57" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="145" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="118" priority="146" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="21" priority="55" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="143" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="116" priority="144" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J5">
+    <cfRule type="cellIs" dxfId="115" priority="107" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="108" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J4">
+    <cfRule type="cellIs" dxfId="113" priority="105" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="106" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J7">
+    <cfRule type="cellIs" dxfId="111" priority="103" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="110" priority="104" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="cellIs" dxfId="109" priority="101" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="102" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K6">
+    <cfRule type="cellIs" dxfId="107" priority="99" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="106" priority="100" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="cellIs" dxfId="105" priority="97" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="104" priority="98" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I12">
+    <cfRule type="cellIs" dxfId="103" priority="95" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="96" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G12">
+    <cfRule type="cellIs" dxfId="101" priority="93" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="100" priority="94" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K12">
+    <cfRule type="cellIs" dxfId="99" priority="91" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="98" priority="92" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M12">
+    <cfRule type="cellIs" dxfId="97" priority="89" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="90" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46">
+    <cfRule type="cellIs" dxfId="95" priority="87" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="94" priority="88" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I47">
+    <cfRule type="cellIs" dxfId="93" priority="85" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="92" priority="86" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H47">
+    <cfRule type="cellIs" dxfId="91" priority="83" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="84" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J48">
+    <cfRule type="cellIs" dxfId="89" priority="81" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="88" priority="82" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J51">
+    <cfRule type="cellIs" dxfId="87" priority="79" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="80" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I49">
+    <cfRule type="cellIs" dxfId="85" priority="77" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="78" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I51">
+    <cfRule type="cellIs" dxfId="83" priority="75" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="76" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H44:J44">
+    <cfRule type="cellIs" dxfId="81" priority="73" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="74" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J36">
+    <cfRule type="cellIs" dxfId="79" priority="71" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="72" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I37">
+    <cfRule type="cellIs" dxfId="77" priority="69" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="70" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H37">
+    <cfRule type="cellIs" dxfId="75" priority="67" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="68" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J38">
+    <cfRule type="cellIs" dxfId="73" priority="65" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="66" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J41">
+    <cfRule type="cellIs" dxfId="71" priority="63" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="64" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I39">
+    <cfRule type="cellIs" dxfId="69" priority="61" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="62" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I41">
+    <cfRule type="cellIs" dxfId="67" priority="59" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="60" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:J34">
+    <cfRule type="cellIs" dxfId="65" priority="57" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="58" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J26">
+    <cfRule type="cellIs" dxfId="63" priority="55" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="56" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I27">
+    <cfRule type="cellIs" dxfId="61" priority="53" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="54" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H27">
+    <cfRule type="cellIs" dxfId="59" priority="51" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="52" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28">
+    <cfRule type="cellIs" dxfId="57" priority="49" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="50" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J31">
+    <cfRule type="cellIs" dxfId="55" priority="47" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="48" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I29">
+    <cfRule type="cellIs" dxfId="53" priority="45" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="46" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I31">
+    <cfRule type="cellIs" dxfId="51" priority="43" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="44" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H24:J24">
+    <cfRule type="cellIs" dxfId="49" priority="41" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="42" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J56">
+    <cfRule type="cellIs" dxfId="47" priority="39" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="40" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I57">
+    <cfRule type="cellIs" dxfId="45" priority="37" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="38" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H57">
+    <cfRule type="cellIs" dxfId="43" priority="35" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="36" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J58">
+    <cfRule type="cellIs" dxfId="41" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="34" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J61">
+    <cfRule type="cellIs" dxfId="39" priority="31" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="32" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I59">
+    <cfRule type="cellIs" dxfId="37" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="36" priority="30" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I61">
+    <cfRule type="cellIs" dxfId="35" priority="27" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="34" priority="28" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54:J54">
+    <cfRule type="cellIs" dxfId="33" priority="25" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="32" priority="26" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K68">
+    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H68">
+    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I68">
+    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J68">
     <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1893,15 +4198,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J4">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
+  <conditionalFormatting sqref="K17">
     <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1909,7 +4206,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J9">
+  <conditionalFormatting sqref="H18:K18">
     <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1917,7 +4214,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6">
+  <conditionalFormatting sqref="H19:K19">
     <cfRule type="cellIs" dxfId="11" priority="11" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1925,7 +4222,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8">
+  <conditionalFormatting sqref="J22">
     <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1933,7 +4230,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
+  <conditionalFormatting sqref="J32">
     <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1941,7 +4238,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G12">
+  <conditionalFormatting sqref="J42">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1949,7 +4246,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
+  <conditionalFormatting sqref="J52">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -1957,7 +4254,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M12">
+  <conditionalFormatting sqref="F68">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
added Pointer and ALU schematic
</commit_message>
<xml_diff>
--- a/CPU in Excel MAIN.xlsx
+++ b/CPU in Excel MAIN.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\100146766\ePU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC55285A-8D12-4B81-8CB9-D660DD05B09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E802606-5803-496B-A388-D867BED88DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,8 +49,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="63">
   <si>
     <t>CLOCK</t>
   </si>
@@ -160,25 +182,85 @@
     <t>2-1 MUX</t>
   </si>
   <si>
-    <t>2-BIT OR</t>
-  </si>
-  <si>
-    <t>BITB1</t>
-  </si>
-  <si>
-    <t>BITB2</t>
-  </si>
-  <si>
-    <t>BITA1</t>
-  </si>
-  <si>
-    <t>BITA2</t>
-  </si>
-  <si>
     <t>4-BIT OR</t>
   </si>
   <si>
     <t>4-BIT AND</t>
+  </si>
+  <si>
+    <t>4-4 AND</t>
+  </si>
+  <si>
+    <t>4-4 OR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OP1 </t>
+  </si>
+  <si>
+    <t>OP2</t>
+  </si>
+  <si>
+    <t>4BITB</t>
+  </si>
+  <si>
+    <t>4BITA</t>
+  </si>
+  <si>
+    <t>MUX</t>
+  </si>
+  <si>
+    <t>ALU</t>
+  </si>
+  <si>
+    <t>ADD/SUB</t>
+  </si>
+  <si>
+    <t>4BIT OUT</t>
+  </si>
+  <si>
+    <t>4-1 OR</t>
+  </si>
+  <si>
+    <t>ZERO</t>
+  </si>
+  <si>
+    <t>NEG</t>
+  </si>
+  <si>
+    <t>SET DELAY</t>
+  </si>
+  <si>
+    <t>DELAY TIMER</t>
+  </si>
+  <si>
+    <t>OUTPUT</t>
+  </si>
+  <si>
+    <t>BITS</t>
+  </si>
+  <si>
+    <t>POINTER</t>
+  </si>
+  <si>
+    <t>ROW REFERENCE</t>
+  </si>
+  <si>
+    <t>COLUMN REFERENCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ARRAY POINTER</t>
+  </si>
+  <si>
+    <t>CELL POINTER</t>
+  </si>
+  <si>
+    <t>POINTER INDEX</t>
+  </si>
+  <si>
+    <t>ARRAY BITS</t>
   </si>
 </sst>
 </file>
@@ -245,7 +327,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="66">
+  <borders count="72">
     <border>
       <left/>
       <right/>
@@ -940,11 +1022,73 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1009,11 +1153,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="3" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1022,8 +1174,19 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1043,264 +1206,26 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="1" fillId="3" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="71" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="406">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFE7E6E6"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF3F3F3F"/>
-          <bgColor rgb="FF3F3F3F"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="382">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -5141,10 +5066,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH72"/>
+  <dimension ref="A1:AH93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="AE56" activeCellId="1" sqref="E29 AE56"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="T100" sqref="T100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" customHeight="1"/>
@@ -5152,7 +5077,7 @@
     <row r="1" spans="1:32" ht="15" customHeight="1">
       <c r="A1" s="1">
         <f ca="1">IF(A1 = 1, 0, IF(A1 = 0, 1))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -5177,7 +5102,7 @@
     <row r="3" spans="1:32" ht="15" customHeight="1">
       <c r="A3" s="1">
         <f ca="1">IF(A1=1, 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
@@ -5197,7 +5122,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="7">
         <f ca="1">IF(CLOCK = 0, J4, IF(AND(CLOCK = 1,INPUT = 1,RESET = 0), 0, IF(AND(CLOCK = 1,INPUT = 0,RESET = 1), 1, IF(AND(CLOCK = 1,INPUT = 0,RESET = 0), J4, IF(AND(CLOCK = 1,INPUT = 1,RESET = 1),IF(JK.1 = 1, 0, 1))))))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="6"/>
       <c r="L4" s="8"/>
@@ -5241,7 +5166,7 @@
     <row r="5" spans="1:32" ht="15" customHeight="1">
       <c r="A5" s="1">
         <f ca="1">IF(A3 = 1, 0, 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -5251,11 +5176,11 @@
       <c r="I5" s="13"/>
       <c r="J5" s="1">
         <f ca="1">IF(CLOCK = 0, J5, IF(AND(CLOCK = 1,JK.1 = 1,JK.1 = 0), 0, IF(AND(CLOCK = 1,JK.1 = 0,JK.1 = 1), 1, IF(AND(CLOCK = 1,JK.1 = 0, JK.1 = 0), J5, IF(AND(CLOCK = 1,JK.1 = 1,JK.1 = 1), IF(JK.2 = 1, 0, 1))))))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K5" s="13"/>
       <c r="L5" s="14"/>
-      <c r="M5" s="48" t="s">
+      <c r="M5" s="63" t="s">
         <v>9</v>
       </c>
       <c r="N5" s="14"/>
@@ -5290,10 +5215,10 @@
       <c r="J6" s="13"/>
       <c r="K6" s="1">
         <f ca="1">IF(AND(JK.1 = 1, JK.2 = 1), 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L6" s="14"/>
-      <c r="M6" s="49"/>
+      <c r="M6" s="64"/>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
       <c r="P6" s="14"/>
@@ -5303,7 +5228,7 @@
       <c r="U6" s="14"/>
       <c r="V6" s="14"/>
       <c r="W6" s="14"/>
-      <c r="X6" s="51" t="s">
+      <c r="X6" s="55" t="s">
         <v>10</v>
       </c>
       <c r="Z6" s="19"/>
@@ -5320,7 +5245,7 @@
     <row r="7" spans="1:32" ht="15" customHeight="1">
       <c r="A7" s="1">
         <f ca="1">IF(AND(A3 = 1, C3 = 1), 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
@@ -5334,7 +5259,7 @@
       </c>
       <c r="K7" s="13"/>
       <c r="L7" s="14"/>
-      <c r="M7" s="50"/>
+      <c r="M7" s="65"/>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
       <c r="P7" s="14"/>
@@ -5347,7 +5272,7 @@
         <v>0</v>
       </c>
       <c r="W7" s="14"/>
-      <c r="X7" s="52"/>
+      <c r="X7" s="56"/>
       <c r="Z7" s="19"/>
       <c r="AA7" s="1">
         <f>IF(AD4 = 1, 0, 1)</f>
@@ -5370,7 +5295,7 @@
       <c r="J8" s="13"/>
       <c r="K8" s="1">
         <f t="array" aca="1" ref="K8" ca="1">IF(AND(AND.1 = 1, JK.3 = 1), 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L8" s="14"/>
       <c r="M8" s="14"/>
@@ -5389,7 +5314,7 @@
       </c>
       <c r="V8" s="13"/>
       <c r="W8" s="14"/>
-      <c r="X8" s="53"/>
+      <c r="X8" s="57"/>
       <c r="Z8" s="19"/>
       <c r="AA8" s="13"/>
       <c r="AB8" s="13"/>
@@ -5399,7 +5324,7 @@
       </c>
       <c r="AD8" s="13"/>
       <c r="AE8" s="18"/>
-      <c r="AF8" s="54" t="s">
+      <c r="AF8" s="58" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5416,7 +5341,7 @@
       <c r="I9" s="13"/>
       <c r="J9" s="1">
         <f ca="1">IF(CLOCK = 0, J9, IF(AND(CLOCK = 1,AND.2 = 1,AND.2 = 0), 0, IF(AND(CLOCK = 1,AND.2 = 0,AND.2 = 1), 1, IF(AND(CLOCK = 1,AND.2 = 0,AND.2 = 0), J9, IF(AND(CLOCK = 1,AND.2 = 1,AND.2 = 1), IF(JK.4 = 1, 0, 1))))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="13"/>
       <c r="L9" s="14"/>
@@ -5443,7 +5368,7 @@
       <c r="AC9" s="13"/>
       <c r="AD9" s="13"/>
       <c r="AE9" s="18"/>
-      <c r="AF9" s="55"/>
+      <c r="AF9" s="51"/>
     </row>
     <row r="10" spans="1:32" ht="15" customHeight="1">
       <c r="A10" s="1"/>
@@ -5476,12 +5401,12 @@
       <c r="AC10" s="13"/>
       <c r="AD10" s="13"/>
       <c r="AE10" s="18"/>
-      <c r="AF10" s="56"/>
+      <c r="AF10" s="54"/>
     </row>
     <row r="11" spans="1:32" ht="15" customHeight="1">
       <c r="A11" s="1">
         <f ca="1">IF(_xlfn.XOR(A3 = 1, C3 = 1), 1, 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
@@ -5515,7 +5440,7 @@
       <c r="A12" s="1"/>
       <c r="G12" s="26">
         <f ca="1">IF(JK.4 = 1, 0, 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>8</v>
@@ -5529,23 +5454,23 @@
       </c>
       <c r="K12" s="1">
         <f ca="1">IF(JK.2 = 1, 0, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="13" t="s">
         <v>8</v>
       </c>
       <c r="M12" s="1">
         <f ca="1">IF(JK.1 = 1, 0, 1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="O12" s="57" t="s">
+      <c r="O12" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="59"/>
+      <c r="P12" s="67"/>
+      <c r="Q12" s="68"/>
       <c r="S12" s="27"/>
       <c r="T12" s="28" t="s">
         <v>4</v>
@@ -5589,9 +5514,9 @@
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
       <c r="N13" s="23"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="61"/>
-      <c r="Q13" s="62"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="70"/>
+      <c r="Q13" s="71"/>
       <c r="Z13" s="17"/>
       <c r="AA13" s="18"/>
       <c r="AB13" s="18"/>
@@ -5604,7 +5529,7 @@
       <c r="A14" s="1"/>
       <c r="G14" s="31">
         <f ca="1">NOT.4</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="28" t="s">
         <v>18</v>
@@ -5618,21 +5543,21 @@
       </c>
       <c r="K14" s="29">
         <f ca="1">NOT.2</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" s="28" t="s">
         <v>20</v>
       </c>
       <c r="M14" s="29">
         <f ca="1">NOT.1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N14" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="O14" s="63"/>
-      <c r="P14" s="64"/>
-      <c r="Q14" s="65"/>
+      <c r="O14" s="72"/>
+      <c r="P14" s="73"/>
+      <c r="Q14" s="74"/>
       <c r="Z14" s="32"/>
       <c r="AA14" s="29">
         <f>AA12</f>
@@ -5654,7 +5579,7 @@
     <row r="15" spans="1:32" ht="15" customHeight="1">
       <c r="A15" s="1">
         <f ca="1">IF(AND(A3 = 1, C3 = 1), 0, 1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
@@ -5679,7 +5604,7 @@
         <v>5</v>
       </c>
       <c r="M16" s="36"/>
-      <c r="N16" s="66" t="s">
+      <c r="N16" s="75" t="s">
         <v>23</v>
       </c>
       <c r="O16" s="9"/>
@@ -5717,7 +5642,7 @@
     <row r="17" spans="1:34" ht="15" customHeight="1">
       <c r="A17" s="1">
         <f ca="1">IF(OR(AND(A3 = 1, C3 = 1), AND(A3 = 0, C3 = 0)), 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>24</v>
@@ -5739,7 +5664,7 @@
         <v>6</v>
       </c>
       <c r="M17" s="18"/>
-      <c r="N17" s="67"/>
+      <c r="N17" s="76"/>
       <c r="O17" s="15"/>
       <c r="Q17" s="16"/>
       <c r="R17" s="14"/>
@@ -5764,7 +5689,7 @@
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
       <c r="M18" s="18"/>
-      <c r="N18" s="68"/>
+      <c r="N18" s="77"/>
       <c r="O18" s="15"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="13"/>
@@ -5775,7 +5700,7 @@
       </c>
       <c r="U18" s="13"/>
       <c r="V18" s="23"/>
-      <c r="W18" s="51" t="s">
+      <c r="W18" s="55" t="s">
         <v>25</v>
       </c>
       <c r="Y18" s="19"/>
@@ -5787,7 +5712,7 @@
       </c>
       <c r="AC18" s="13"/>
       <c r="AD18" s="23"/>
-      <c r="AE18" s="69" t="s">
+      <c r="AE18" s="78" t="s">
         <v>26</v>
       </c>
     </row>
@@ -5814,7 +5739,7 @@
       <c r="T19" s="13"/>
       <c r="U19" s="13"/>
       <c r="V19" s="23"/>
-      <c r="W19" s="52"/>
+      <c r="W19" s="56"/>
       <c r="Y19" s="19"/>
       <c r="Z19" s="1">
         <f>IF(Z16 = 1, 0, 1)</f>
@@ -5824,7 +5749,7 @@
       <c r="AB19" s="13"/>
       <c r="AC19" s="13"/>
       <c r="AD19" s="23"/>
-      <c r="AE19" s="55"/>
+      <c r="AE19" s="51"/>
     </row>
     <row r="20" spans="1:34" ht="15" customHeight="1">
       <c r="G20" s="17"/>
@@ -5859,19 +5784,19 @@
       <c r="T20" s="13"/>
       <c r="U20" s="13"/>
       <c r="V20" s="23"/>
-      <c r="W20" s="53"/>
+      <c r="W20" s="57"/>
       <c r="Y20" s="19"/>
       <c r="Z20" s="13"/>
       <c r="AA20" s="13"/>
       <c r="AB20" s="13"/>
       <c r="AC20" s="13"/>
       <c r="AD20" s="23"/>
-      <c r="AE20" s="70"/>
+      <c r="AE20" s="52"/>
     </row>
     <row r="21" spans="1:34" ht="15" customHeight="1">
       <c r="A21" s="1">
         <f ca="1">IF(A1 = 0, A21, IF(AND(A1 = 1, C1 = 1, E1 = 0), 1, IF(AND(A1 = 1, C1 = 0, E1 = 1), 0, IF(AND(A1 = 1, C1 = 0, E1 = 0), A21, IF(AND(A1 = 1, C1 = 1, E1 = 1), IF(A21 = 1, 0, 1))))))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>28</v>
@@ -5993,7 +5918,7 @@
       </c>
       <c r="L24" s="13"/>
       <c r="M24" s="18"/>
-      <c r="N24" s="54" t="s">
+      <c r="N24" s="58" t="s">
         <v>12</v>
       </c>
       <c r="O24" s="15"/>
@@ -6009,7 +5934,7 @@
       <c r="K25" s="13"/>
       <c r="L25" s="13"/>
       <c r="M25" s="18"/>
-      <c r="N25" s="55"/>
+      <c r="N25" s="51"/>
       <c r="O25" s="15"/>
       <c r="Q25" s="34"/>
       <c r="R25" s="35">
@@ -6066,7 +5991,7 @@
       <c r="K26" s="13"/>
       <c r="L26" s="13"/>
       <c r="M26" s="18"/>
-      <c r="N26" s="56"/>
+      <c r="N26" s="54"/>
       <c r="O26" s="15"/>
       <c r="Q26" s="17"/>
       <c r="R26" s="3">
@@ -6125,7 +6050,7 @@
       <c r="AE27" s="13"/>
       <c r="AF27" s="13"/>
       <c r="AG27" s="23"/>
-      <c r="AH27" s="76" t="s">
+      <c r="AH27" s="50" t="s">
         <v>35</v>
       </c>
     </row>
@@ -6155,7 +6080,7 @@
       </c>
       <c r="W28" s="18"/>
       <c r="X28" s="18"/>
-      <c r="Y28" s="75" t="s">
+      <c r="Y28" s="53" t="s">
         <v>30</v>
       </c>
       <c r="AA28" s="19"/>
@@ -6171,7 +6096,7 @@
       </c>
       <c r="AF28" s="13"/>
       <c r="AG28" s="23"/>
-      <c r="AH28" s="55"/>
+      <c r="AH28" s="51"/>
     </row>
     <row r="29" spans="1:34" ht="15" customHeight="1">
       <c r="G29" s="17"/>
@@ -6197,7 +6122,7 @@
       <c r="V29" s="8"/>
       <c r="W29" s="9"/>
       <c r="X29" s="18"/>
-      <c r="Y29" s="55"/>
+      <c r="Y29" s="51"/>
       <c r="AA29" s="19"/>
       <c r="AB29" s="23"/>
       <c r="AC29" s="3">
@@ -6208,7 +6133,7 @@
       <c r="AE29" s="13"/>
       <c r="AF29" s="13"/>
       <c r="AG29" s="23"/>
-      <c r="AH29" s="70"/>
+      <c r="AH29" s="52"/>
     </row>
     <row r="30" spans="1:34" ht="15" customHeight="1">
       <c r="G30" s="17"/>
@@ -6247,7 +6172,7 @@
       <c r="V30" s="14"/>
       <c r="W30" s="15"/>
       <c r="X30" s="18"/>
-      <c r="Y30" s="56"/>
+      <c r="Y30" s="54"/>
       <c r="AA30" s="19"/>
       <c r="AB30" s="23"/>
       <c r="AC30" s="23"/>
@@ -6273,14 +6198,14 @@
       <c r="T31" s="14"/>
       <c r="U31" s="14"/>
       <c r="V31" s="14"/>
-      <c r="W31" s="51" t="s">
+      <c r="W31" s="55" t="s">
         <v>10</v>
       </c>
       <c r="X31" s="18"/>
       <c r="Y31" s="15"/>
       <c r="AA31" s="42"/>
       <c r="AB31" s="41"/>
-      <c r="AC31" s="77">
+      <c r="AC31" s="48">
         <f>AC29</f>
         <v>0</v>
       </c>
@@ -6326,7 +6251,7 @@
         <v>0</v>
       </c>
       <c r="V32" s="14"/>
-      <c r="W32" s="52"/>
+      <c r="W32" s="56"/>
       <c r="X32" s="18"/>
       <c r="Y32" s="15"/>
     </row>
@@ -6352,23 +6277,26 @@
       </c>
       <c r="U33" s="13"/>
       <c r="V33" s="14"/>
-      <c r="W33" s="53"/>
+      <c r="W33" s="57"/>
       <c r="X33" s="18"/>
       <c r="Y33" s="15"/>
       <c r="AA33" s="37"/>
-      <c r="AB33" s="78" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC33" s="78" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD33" s="78" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE33" s="78" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF33" s="38"/>
+      <c r="AB33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF33" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG33" s="38"/>
     </row>
     <row r="34" spans="7:33" ht="15" customHeight="1">
       <c r="G34" s="17"/>
@@ -6397,7 +6325,7 @@
       <c r="Y34" s="15"/>
       <c r="AA34" s="19"/>
       <c r="AB34" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC34" s="3">
         <v>0</v>
@@ -6408,7 +6336,10 @@
       <c r="AE34" s="3">
         <v>0</v>
       </c>
-      <c r="AF34" s="39"/>
+      <c r="AF34" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG34" s="39"/>
     </row>
     <row r="35" spans="7:33" ht="15" customHeight="1">
       <c r="G35" s="17"/>
@@ -6443,7 +6374,8 @@
       <c r="AC35" s="23"/>
       <c r="AD35" s="23"/>
       <c r="AE35" s="23"/>
-      <c r="AF35" s="76" t="s">
+      <c r="AF35" s="23"/>
+      <c r="AG35" s="79" t="s">
         <v>36</v>
       </c>
     </row>
@@ -6458,7 +6390,7 @@
       </c>
       <c r="L36" s="13"/>
       <c r="M36" s="18"/>
-      <c r="N36" s="54" t="s">
+      <c r="N36" s="58" t="s">
         <v>12</v>
       </c>
       <c r="O36" s="15"/>
@@ -6473,16 +6405,23 @@
       <c r="Y36" s="15"/>
       <c r="AA36" s="19"/>
       <c r="AB36" s="3">
-        <f>IF(OR(AB34 = 1, AD34 =1), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="AC36" s="13"/>
+        <f>IF(OR(AB33 = 1, AB34 =1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC36" s="3">
+        <f>IF(OR(AC33 = 1, AC34 =1), 1, 0)</f>
+        <v>0</v>
+      </c>
       <c r="AD36" s="3">
-        <f>IF(OR(AC34 = 1, AE34 =1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE36" s="23"/>
-      <c r="AF36" s="55"/>
+        <f>IF(OR(AD33 = 1, AD34 =1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE36" s="3">
+        <f>IF(OR(AE33 = 1, AE34 =1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AF36" s="23"/>
+      <c r="AG36" s="79"/>
     </row>
     <row r="37" spans="7:33" ht="15" customHeight="1">
       <c r="G37" s="17"/>
@@ -6495,7 +6434,7 @@
       <c r="K37" s="13"/>
       <c r="L37" s="13"/>
       <c r="M37" s="18"/>
-      <c r="N37" s="55"/>
+      <c r="N37" s="51"/>
       <c r="O37" s="15"/>
       <c r="Q37" s="17"/>
       <c r="R37" s="27"/>
@@ -6517,14 +6456,12 @@
       <c r="X37" s="18"/>
       <c r="Y37" s="15"/>
       <c r="AA37" s="19"/>
-      <c r="AB37" s="13"/>
-      <c r="AC37" s="3">
-        <f>IF(OR(AB36 = 1, AD36 =1), 1, 0)</f>
-        <v>1</v>
-      </c>
-      <c r="AD37" s="13"/>
+      <c r="AB37" s="23"/>
+      <c r="AC37" s="23"/>
+      <c r="AD37" s="23"/>
       <c r="AE37" s="23"/>
-      <c r="AF37" s="70"/>
+      <c r="AF37" s="23"/>
+      <c r="AG37" s="79"/>
     </row>
     <row r="38" spans="7:33" ht="15" customHeight="1">
       <c r="G38" s="17"/>
@@ -6537,7 +6474,7 @@
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
       <c r="M38" s="18"/>
-      <c r="N38" s="56"/>
+      <c r="N38" s="54"/>
       <c r="O38" s="15"/>
       <c r="Q38" s="17"/>
       <c r="R38" s="18"/>
@@ -6553,12 +6490,27 @@
       <c r="W38" s="18"/>
       <c r="X38" s="18"/>
       <c r="Y38" s="15"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="23"/>
-      <c r="AC38" s="23"/>
-      <c r="AD38" s="23"/>
-      <c r="AE38" s="23"/>
-      <c r="AF38" s="39"/>
+      <c r="AA38" s="42"/>
+      <c r="AB38" s="48">
+        <f>AB36</f>
+        <v>0</v>
+      </c>
+      <c r="AC38" s="48">
+        <f>AC36</f>
+        <v>0</v>
+      </c>
+      <c r="AD38" s="48">
+        <f>AD36</f>
+        <v>0</v>
+      </c>
+      <c r="AE38" s="48">
+        <f>AE36</f>
+        <v>0</v>
+      </c>
+      <c r="AF38" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG38" s="43"/>
     </row>
     <row r="39" spans="7:33" ht="15" customHeight="1">
       <c r="G39" s="17"/>
@@ -6585,17 +6537,6 @@
       <c r="W39" s="9"/>
       <c r="X39" s="18"/>
       <c r="Y39" s="15"/>
-      <c r="AA39" s="42"/>
-      <c r="AB39" s="41"/>
-      <c r="AC39" s="77">
-        <f>AC37</f>
-        <v>1</v>
-      </c>
-      <c r="AD39" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="AE39" s="41"/>
-      <c r="AF39" s="43"/>
     </row>
     <row r="40" spans="7:33" ht="15" customHeight="1">
       <c r="G40" s="17"/>
@@ -6628,6 +6569,23 @@
       <c r="W40" s="15"/>
       <c r="X40" s="18"/>
       <c r="Y40" s="15"/>
+      <c r="AA40" s="37"/>
+      <c r="AB40" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="3">
+        <v>0</v>
+      </c>
+      <c r="AD40" s="3">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF40" s="49" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG40" s="38"/>
     </row>
     <row r="41" spans="7:33" ht="15" customHeight="1">
       <c r="G41" s="17"/>
@@ -6645,12 +6603,12 @@
       <c r="T41" s="14"/>
       <c r="U41" s="14"/>
       <c r="V41" s="14"/>
-      <c r="W41" s="51" t="s">
+      <c r="W41" s="55" t="s">
         <v>10</v>
       </c>
       <c r="X41" s="18"/>
       <c r="Y41" s="15"/>
-      <c r="AA41" s="37"/>
+      <c r="AA41" s="19"/>
       <c r="AB41" s="3">
         <v>0</v>
       </c>
@@ -6663,10 +6621,10 @@
       <c r="AE41" s="3">
         <v>0</v>
       </c>
-      <c r="AF41" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG41" s="38"/>
+      <c r="AF41" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="AG41" s="39"/>
     </row>
     <row r="42" spans="7:33" ht="15" customHeight="1">
       <c r="G42" s="17"/>
@@ -6697,26 +6655,18 @@
         <v>0</v>
       </c>
       <c r="V42" s="14"/>
-      <c r="W42" s="52"/>
+      <c r="W42" s="56"/>
       <c r="X42" s="18"/>
       <c r="Y42" s="15"/>
       <c r="AA42" s="19"/>
-      <c r="AB42" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC42" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD42" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE42" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF42" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG42" s="39"/>
+      <c r="AB42" s="23"/>
+      <c r="AC42" s="23"/>
+      <c r="AD42" s="23"/>
+      <c r="AE42" s="23"/>
+      <c r="AF42" s="23"/>
+      <c r="AG42" s="80" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="43" spans="7:33" ht="15" customHeight="1">
       <c r="G43" s="17"/>
@@ -6740,18 +6690,28 @@
       </c>
       <c r="U43" s="13"/>
       <c r="V43" s="14"/>
-      <c r="W43" s="53"/>
+      <c r="W43" s="57"/>
       <c r="X43" s="18"/>
       <c r="Y43" s="15"/>
       <c r="AA43" s="19"/>
-      <c r="AB43" s="23"/>
-      <c r="AC43" s="23"/>
-      <c r="AD43" s="23"/>
-      <c r="AE43" s="23"/>
+      <c r="AB43" s="3">
+        <f>IF(AND(AB40 = 1, AB41 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AC43" s="3">
+        <f>IF(AND(AC40 = 1, AC41 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AD43" s="3">
+        <f>IF(AND(AD40 = 1, AD41 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AE43" s="3">
+        <f>IF(AND(AE40 = 1, AE41 = 1), 1, 0)</f>
+        <v>0</v>
+      </c>
       <c r="AF43" s="23"/>
-      <c r="AG43" s="80" t="s">
-        <v>41</v>
-      </c>
+      <c r="AG43" s="80"/>
     </row>
     <row r="44" spans="7:33" ht="15" customHeight="1">
       <c r="G44" s="17"/>
@@ -6791,22 +6751,10 @@
       <c r="X44" s="18"/>
       <c r="Y44" s="15"/>
       <c r="AA44" s="19"/>
-      <c r="AB44" s="3">
-        <f>IF(OR(AB41 = 1, AB42 =1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC44" s="3">
-        <f>IF(OR(AC41 = 1, AC42 =1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD44" s="3">
-        <f>IF(OR(AD41 = 1, AD42 =1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE44" s="3">
-        <f>IF(OR(AE41 = 1, AE42 =1), 1, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="AB44" s="23"/>
+      <c r="AC44" s="23"/>
+      <c r="AD44" s="23"/>
+      <c r="AE44" s="23"/>
       <c r="AF44" s="23"/>
       <c r="AG44" s="80"/>
     </row>
@@ -6832,13 +6780,27 @@
       <c r="W45" s="15"/>
       <c r="X45" s="18"/>
       <c r="Y45" s="15"/>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="23"/>
-      <c r="AC45" s="23"/>
-      <c r="AD45" s="23"/>
-      <c r="AE45" s="23"/>
-      <c r="AF45" s="23"/>
-      <c r="AG45" s="80"/>
+      <c r="AA45" s="42"/>
+      <c r="AB45" s="48">
+        <f>AB43</f>
+        <v>0</v>
+      </c>
+      <c r="AC45" s="48">
+        <f>AC43</f>
+        <v>0</v>
+      </c>
+      <c r="AD45" s="48">
+        <f>AD43</f>
+        <v>0</v>
+      </c>
+      <c r="AE45" s="48">
+        <f>AE43</f>
+        <v>0</v>
+      </c>
+      <c r="AF45" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="AG45" s="43"/>
     </row>
     <row r="46" spans="7:33" ht="15" customHeight="1">
       <c r="G46" s="17"/>
@@ -6862,27 +6824,6 @@
       <c r="W46" s="15"/>
       <c r="X46" s="18"/>
       <c r="Y46" s="15"/>
-      <c r="AA46" s="42"/>
-      <c r="AB46" s="77">
-        <f>AB44</f>
-        <v>0</v>
-      </c>
-      <c r="AC46" s="77">
-        <f>AC44</f>
-        <v>0</v>
-      </c>
-      <c r="AD46" s="77">
-        <f>AD44</f>
-        <v>0</v>
-      </c>
-      <c r="AE46" s="77">
-        <f>AE44</f>
-        <v>0</v>
-      </c>
-      <c r="AF46" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG46" s="43"/>
     </row>
     <row r="47" spans="7:33" ht="15" customHeight="1">
       <c r="G47" s="17"/>
@@ -6931,7 +6872,7 @@
       </c>
       <c r="L48" s="13"/>
       <c r="M48" s="18"/>
-      <c r="N48" s="54" t="s">
+      <c r="N48" s="58" t="s">
         <v>12</v>
       </c>
       <c r="O48" s="15"/>
@@ -6949,25 +6890,8 @@
       <c r="W48" s="18"/>
       <c r="X48" s="18"/>
       <c r="Y48" s="15"/>
-      <c r="AA48" s="37"/>
-      <c r="AB48" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC48" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD48" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE48" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF48" s="78" t="s">
-        <v>5</v>
-      </c>
-      <c r="AG48" s="38"/>
-    </row>
-    <row r="49" spans="7:33" ht="15" customHeight="1">
+    </row>
+    <row r="49" spans="7:25" ht="15" customHeight="1">
       <c r="G49" s="17"/>
       <c r="H49" s="19"/>
       <c r="I49" s="1">
@@ -6978,7 +6902,7 @@
       <c r="K49" s="13"/>
       <c r="L49" s="13"/>
       <c r="M49" s="18"/>
-      <c r="N49" s="55"/>
+      <c r="N49" s="51"/>
       <c r="O49" s="15"/>
       <c r="Q49" s="17"/>
       <c r="R49" s="4"/>
@@ -6995,25 +6919,8 @@
       <c r="W49" s="9"/>
       <c r="X49" s="18"/>
       <c r="Y49" s="15"/>
-      <c r="AA49" s="19"/>
-      <c r="AB49" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC49" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD49" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE49" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF49" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="AG49" s="39"/>
-    </row>
-    <row r="50" spans="7:33" ht="15" customHeight="1">
+    </row>
+    <row r="50" spans="7:25" ht="15" customHeight="1">
       <c r="G50" s="17"/>
       <c r="H50" s="19"/>
       <c r="I50" s="13"/>
@@ -7024,7 +6931,7 @@
       <c r="K50" s="13"/>
       <c r="L50" s="13"/>
       <c r="M50" s="18"/>
-      <c r="N50" s="56"/>
+      <c r="N50" s="54"/>
       <c r="O50" s="15"/>
       <c r="Q50" s="17"/>
       <c r="R50" s="16"/>
@@ -7044,17 +6951,8 @@
       <c r="W50" s="15"/>
       <c r="X50" s="18"/>
       <c r="Y50" s="15"/>
-      <c r="AA50" s="19"/>
-      <c r="AB50" s="23"/>
-      <c r="AC50" s="23"/>
-      <c r="AD50" s="23"/>
-      <c r="AE50" s="23"/>
-      <c r="AF50" s="23"/>
-      <c r="AG50" s="79" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="51" spans="7:33" ht="15" customHeight="1">
+    </row>
+    <row r="51" spans="7:25" ht="15" customHeight="1">
       <c r="G51" s="17"/>
       <c r="H51" s="19"/>
       <c r="I51" s="13"/>
@@ -7070,32 +6968,13 @@
       <c r="T51" s="14"/>
       <c r="U51" s="14"/>
       <c r="V51" s="14"/>
-      <c r="W51" s="51" t="s">
+      <c r="W51" s="55" t="s">
         <v>10</v>
       </c>
       <c r="X51" s="18"/>
       <c r="Y51" s="15"/>
-      <c r="AA51" s="19"/>
-      <c r="AB51" s="3">
-        <f>IF(AND(AB48 = 1, AB49 = 1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AC51" s="3">
-        <f>IF(AND(AC48 = 1, AC49 = 1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AD51" s="3">
-        <f>IF(AND(AD48 = 1, AD49 = 1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AE51" s="3">
-        <f>IF(AND(AE48 = 1, AE49 = 1), 1, 0)</f>
-        <v>0</v>
-      </c>
-      <c r="AF51" s="23"/>
-      <c r="AG51" s="79"/>
-    </row>
-    <row r="52" spans="7:33" ht="15" customHeight="1">
+    </row>
+    <row r="52" spans="7:25" ht="15" customHeight="1">
       <c r="G52" s="17"/>
       <c r="H52" s="19"/>
       <c r="I52" s="1">
@@ -7117,18 +6996,11 @@
         <v>0</v>
       </c>
       <c r="V52" s="14"/>
-      <c r="W52" s="52"/>
+      <c r="W52" s="56"/>
       <c r="X52" s="18"/>
       <c r="Y52" s="15"/>
-      <c r="AA52" s="19"/>
-      <c r="AB52" s="23"/>
-      <c r="AC52" s="23"/>
-      <c r="AD52" s="23"/>
-      <c r="AE52" s="23"/>
-      <c r="AF52" s="23"/>
-      <c r="AG52" s="79"/>
-    </row>
-    <row r="53" spans="7:33" ht="15" customHeight="1">
+    </row>
+    <row r="53" spans="7:25" ht="15" customHeight="1">
       <c r="G53" s="17"/>
       <c r="H53" s="17"/>
       <c r="I53" s="18"/>
@@ -7150,32 +7022,11 @@
       </c>
       <c r="U53" s="13"/>
       <c r="V53" s="14"/>
-      <c r="W53" s="53"/>
+      <c r="W53" s="57"/>
       <c r="X53" s="18"/>
       <c r="Y53" s="15"/>
-      <c r="AA53" s="42"/>
-      <c r="AB53" s="77">
-        <f>AB51</f>
-        <v>0</v>
-      </c>
-      <c r="AC53" s="77">
-        <f>AC51</f>
-        <v>0</v>
-      </c>
-      <c r="AD53" s="77">
-        <f>AD51</f>
-        <v>0</v>
-      </c>
-      <c r="AE53" s="77">
-        <f>AE51</f>
-        <v>0</v>
-      </c>
-      <c r="AF53" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="AG53" s="43"/>
-    </row>
-    <row r="54" spans="7:33" ht="15" customHeight="1">
+    </row>
+    <row r="54" spans="7:25" ht="15" customHeight="1">
       <c r="G54" s="17"/>
       <c r="H54" s="32"/>
       <c r="I54" s="29">
@@ -7208,7 +7059,7 @@
       <c r="X54" s="18"/>
       <c r="Y54" s="15"/>
     </row>
-    <row r="55" spans="7:33" ht="15" customHeight="1">
+    <row r="55" spans="7:25" ht="15" customHeight="1">
       <c r="G55" s="17"/>
       <c r="H55" s="18"/>
       <c r="I55" s="18"/>
@@ -7231,7 +7082,7 @@
       <c r="X55" s="18"/>
       <c r="Y55" s="15"/>
     </row>
-    <row r="56" spans="7:33" ht="15" customHeight="1">
+    <row r="56" spans="7:25" ht="15" customHeight="1">
       <c r="G56" s="17"/>
       <c r="H56" s="10">
         <f>I54</f>
@@ -7266,7 +7117,7 @@
       <c r="X56" s="18"/>
       <c r="Y56" s="15"/>
     </row>
-    <row r="57" spans="7:33" ht="15" customHeight="1">
+    <row r="57" spans="7:25" ht="15" customHeight="1">
       <c r="G57" s="17"/>
       <c r="H57" s="45"/>
       <c r="I57" s="18"/>
@@ -7296,7 +7147,7 @@
       <c r="X57" s="18"/>
       <c r="Y57" s="15"/>
     </row>
-    <row r="58" spans="7:33" ht="15" customHeight="1">
+    <row r="58" spans="7:25" ht="15" customHeight="1">
       <c r="G58" s="17"/>
       <c r="H58" s="19"/>
       <c r="I58" s="13"/>
@@ -7324,7 +7175,7 @@
       <c r="X58" s="18"/>
       <c r="Y58" s="15"/>
     </row>
-    <row r="59" spans="7:33" ht="15" customHeight="1">
+    <row r="59" spans="7:25" ht="15" customHeight="1">
       <c r="G59" s="17"/>
       <c r="H59" s="19"/>
       <c r="I59" s="1">
@@ -7356,7 +7207,7 @@
       <c r="X59" s="18"/>
       <c r="Y59" s="15"/>
     </row>
-    <row r="60" spans="7:33" ht="15" customHeight="1">
+    <row r="60" spans="7:25" ht="15" customHeight="1">
       <c r="G60" s="17"/>
       <c r="H60" s="19"/>
       <c r="I60" s="13"/>
@@ -7367,7 +7218,7 @@
       </c>
       <c r="L60" s="13"/>
       <c r="M60" s="18"/>
-      <c r="N60" s="54" t="s">
+      <c r="N60" s="58" t="s">
         <v>12</v>
       </c>
       <c r="O60" s="15"/>
@@ -7390,7 +7241,7 @@
       <c r="X60" s="18"/>
       <c r="Y60" s="15"/>
     </row>
-    <row r="61" spans="7:33" ht="15" customHeight="1">
+    <row r="61" spans="7:25" ht="15" customHeight="1">
       <c r="G61" s="17"/>
       <c r="H61" s="19"/>
       <c r="I61" s="1">
@@ -7401,7 +7252,7 @@
       <c r="K61" s="13"/>
       <c r="L61" s="13"/>
       <c r="M61" s="18"/>
-      <c r="N61" s="55"/>
+      <c r="N61" s="51"/>
       <c r="O61" s="15"/>
       <c r="Q61" s="17"/>
       <c r="R61" s="16"/>
@@ -7409,13 +7260,13 @@
       <c r="T61" s="14"/>
       <c r="U61" s="14"/>
       <c r="V61" s="14"/>
-      <c r="W61" s="51" t="s">
+      <c r="W61" s="55" t="s">
         <v>10</v>
       </c>
       <c r="X61" s="18"/>
       <c r="Y61" s="15"/>
     </row>
-    <row r="62" spans="7:33" ht="15" customHeight="1">
+    <row r="62" spans="7:25" ht="15" customHeight="1">
       <c r="G62" s="17"/>
       <c r="H62" s="19"/>
       <c r="I62" s="13"/>
@@ -7426,7 +7277,7 @@
       <c r="K62" s="13"/>
       <c r="L62" s="13"/>
       <c r="M62" s="18"/>
-      <c r="N62" s="56"/>
+      <c r="N62" s="54"/>
       <c r="O62" s="15"/>
       <c r="Q62" s="17"/>
       <c r="R62" s="16"/>
@@ -7437,11 +7288,11 @@
         <v>0</v>
       </c>
       <c r="V62" s="14"/>
-      <c r="W62" s="52"/>
+      <c r="W62" s="56"/>
       <c r="X62" s="18"/>
       <c r="Y62" s="15"/>
     </row>
-    <row r="63" spans="7:33" ht="15" customHeight="1">
+    <row r="63" spans="7:25" ht="15" customHeight="1">
       <c r="G63" s="17"/>
       <c r="H63" s="19"/>
       <c r="I63" s="13"/>
@@ -7463,11 +7314,11 @@
       </c>
       <c r="U63" s="13"/>
       <c r="V63" s="14"/>
-      <c r="W63" s="53"/>
+      <c r="W63" s="57"/>
       <c r="X63" s="18"/>
       <c r="Y63" s="15"/>
     </row>
-    <row r="64" spans="7:33" ht="15" customHeight="1">
+    <row r="64" spans="7:25" ht="15" customHeight="1">
       <c r="G64" s="17"/>
       <c r="H64" s="19"/>
       <c r="I64" s="1">
@@ -7493,7 +7344,7 @@
       <c r="X64" s="18"/>
       <c r="Y64" s="15"/>
     </row>
-    <row r="65" spans="7:25" ht="15" customHeight="1">
+    <row r="65" spans="4:25" ht="15" customHeight="1">
       <c r="G65" s="17"/>
       <c r="H65" s="46"/>
       <c r="I65" s="18"/>
@@ -7516,7 +7367,7 @@
       <c r="X65" s="18"/>
       <c r="Y65" s="15"/>
     </row>
-    <row r="66" spans="7:25" ht="15" customHeight="1">
+    <row r="66" spans="4:25" ht="15" customHeight="1">
       <c r="G66" s="17"/>
       <c r="H66" s="32"/>
       <c r="I66" s="29">
@@ -7546,7 +7397,7 @@
       <c r="X66" s="18"/>
       <c r="Y66" s="15"/>
     </row>
-    <row r="67" spans="7:25" ht="15" customHeight="1">
+    <row r="67" spans="4:25" ht="15" customHeight="1">
       <c r="G67" s="17"/>
       <c r="H67" s="18"/>
       <c r="I67" s="18"/>
@@ -7576,7 +7427,7 @@
       <c r="X67" s="18"/>
       <c r="Y67" s="15"/>
     </row>
-    <row r="68" spans="7:25" ht="15" customHeight="1">
+    <row r="68" spans="4:25" ht="15" customHeight="1">
       <c r="G68" s="32"/>
       <c r="H68" s="29">
         <f>I66</f>
@@ -7615,7 +7466,7 @@
       <c r="X68" s="18"/>
       <c r="Y68" s="15"/>
     </row>
-    <row r="69" spans="7:25" ht="15" customHeight="1">
+    <row r="69" spans="4:25" ht="15" customHeight="1">
       <c r="Q69" s="17"/>
       <c r="R69" s="18"/>
       <c r="S69" s="18"/>
@@ -7626,7 +7477,7 @@
       <c r="X69" s="18"/>
       <c r="Y69" s="15"/>
     </row>
-    <row r="70" spans="7:25" ht="15" customHeight="1">
+    <row r="70" spans="4:25" ht="15" customHeight="1">
       <c r="Q70" s="17"/>
       <c r="R70" s="18"/>
       <c r="S70" s="18"/>
@@ -7637,32 +7488,32 @@
       <c r="X70" s="18"/>
       <c r="Y70" s="15"/>
     </row>
-    <row r="71" spans="7:25" ht="15" customHeight="1">
+    <row r="71" spans="4:25" ht="15" customHeight="1">
       <c r="Q71" s="17"/>
       <c r="R71" s="1">
         <f>IF(_xlfn.XOR(T67 = 1, T57 = 1), 1, 0)</f>
         <v>0</v>
       </c>
-      <c r="S71" s="71" t="s">
+      <c r="S71" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="T71" s="72"/>
+      <c r="T71" s="60"/>
       <c r="U71" s="18"/>
       <c r="V71" s="18"/>
       <c r="W71" s="18"/>
       <c r="X71" s="18"/>
       <c r="Y71" s="15"/>
     </row>
-    <row r="72" spans="7:25" ht="15" customHeight="1">
+    <row r="72" spans="4:25" ht="15" customHeight="1">
       <c r="Q72" s="32"/>
       <c r="R72" s="29">
         <f>T67</f>
         <v>0</v>
       </c>
-      <c r="S72" s="73" t="s">
+      <c r="S72" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="T72" s="74"/>
+      <c r="T72" s="62"/>
       <c r="U72" s="29">
         <f>U67</f>
         <v>0</v>
@@ -7683,23 +7534,374 @@
         <v>31</v>
       </c>
     </row>
+    <row r="79" spans="4:25" ht="15" customHeight="1">
+      <c r="D79" t="s">
+        <v>45</v>
+      </c>
+      <c r="N79" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="80" spans="4:25" ht="15" customHeight="1">
+      <c r="D80" s="81"/>
+      <c r="E80" s="82"/>
+      <c r="F80" s="82"/>
+      <c r="G80" s="82"/>
+      <c r="H80" s="82"/>
+      <c r="I80" s="82"/>
+      <c r="J80" s="82" t="s">
+        <v>42</v>
+      </c>
+      <c r="K80" s="82"/>
+      <c r="L80" s="83" t="s">
+        <v>43</v>
+      </c>
+      <c r="N80" s="81"/>
+      <c r="O80" s="82"/>
+      <c r="P80" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q80" s="82"/>
+      <c r="R80" s="82"/>
+      <c r="S80" s="82"/>
+      <c r="T80" s="82"/>
+      <c r="U80" s="82"/>
+      <c r="V80" s="82"/>
+      <c r="W80" s="82"/>
+      <c r="X80" s="83"/>
+    </row>
+    <row r="81" spans="4:24" ht="15" customHeight="1">
+      <c r="D81" s="84"/>
+      <c r="E81" s="85"/>
+      <c r="F81" s="85"/>
+      <c r="G81" s="85"/>
+      <c r="H81" s="85"/>
+      <c r="I81" s="85"/>
+      <c r="J81" s="85"/>
+      <c r="K81" s="85"/>
+      <c r="L81" s="86"/>
+      <c r="N81" s="84"/>
+      <c r="O81" s="85"/>
+      <c r="P81" s="85">
+        <v>1</v>
+      </c>
+      <c r="Q81" s="85">
+        <v>0</v>
+      </c>
+      <c r="R81" s="85">
+        <v>1</v>
+      </c>
+      <c r="S81" s="85">
+        <v>1</v>
+      </c>
+      <c r="T81" s="85" t="s">
+        <v>58</v>
+      </c>
+      <c r="U81" s="85"/>
+      <c r="V81" s="85" cm="1">
+        <f t="array" aca="1" ref="V81" ca="1">INDIRECT(ADDRESS(U84, U83 + R85))</f>
+        <v>1</v>
+      </c>
+      <c r="W81" s="85" t="s">
+        <v>59</v>
+      </c>
+      <c r="X81" s="86"/>
+    </row>
+    <row r="82" spans="4:24" ht="15" customHeight="1">
+      <c r="D82" s="84"/>
+      <c r="E82" s="85"/>
+      <c r="F82" s="85"/>
+      <c r="G82" s="85"/>
+      <c r="H82" s="85"/>
+      <c r="I82" s="85"/>
+      <c r="J82" s="85"/>
+      <c r="K82" s="85"/>
+      <c r="L82" s="86"/>
+      <c r="N82" s="84"/>
+      <c r="O82" s="85"/>
+      <c r="P82" s="85"/>
+      <c r="Q82" s="85"/>
+      <c r="R82" s="85"/>
+      <c r="S82" s="85"/>
+      <c r="T82" s="85"/>
+      <c r="U82" s="85"/>
+      <c r="V82" s="85"/>
+      <c r="W82" s="85"/>
+      <c r="X82" s="86"/>
+    </row>
+    <row r="83" spans="4:24" ht="15" customHeight="1">
+      <c r="D83" s="84"/>
+      <c r="E83" s="85"/>
+      <c r="F83" s="85"/>
+      <c r="G83" s="85" t="s">
+        <v>46</v>
+      </c>
+      <c r="H83" s="85"/>
+      <c r="I83" s="85" t="s">
+        <v>39</v>
+      </c>
+      <c r="J83" s="85"/>
+      <c r="K83" s="85" t="s">
+        <v>38</v>
+      </c>
+      <c r="L83" s="86"/>
+      <c r="N83" s="84"/>
+      <c r="O83" s="85"/>
+      <c r="P83" s="85">
+        <v>1010</v>
+      </c>
+      <c r="Q83" s="85" t="s">
+        <v>54</v>
+      </c>
+      <c r="R83" s="85"/>
+      <c r="S83" s="85"/>
+      <c r="T83" s="85"/>
+      <c r="U83" s="85">
+        <v>15</v>
+      </c>
+      <c r="V83" s="85" t="s">
+        <v>56</v>
+      </c>
+      <c r="W83" s="85"/>
+      <c r="X83" s="86"/>
+    </row>
+    <row r="84" spans="4:24" ht="15" customHeight="1">
+      <c r="D84" s="84"/>
+      <c r="E84" s="85"/>
+      <c r="F84" s="85"/>
+      <c r="G84" s="85"/>
+      <c r="H84" s="85"/>
+      <c r="I84" s="85"/>
+      <c r="J84" s="85"/>
+      <c r="K84" s="85"/>
+      <c r="L84" s="86"/>
+      <c r="N84" s="84"/>
+      <c r="O84" s="85"/>
+      <c r="P84" s="85"/>
+      <c r="Q84" s="85"/>
+      <c r="R84" s="85"/>
+      <c r="S84" s="85"/>
+      <c r="T84" s="85"/>
+      <c r="U84" s="85">
+        <v>81</v>
+      </c>
+      <c r="V84" s="85" t="s">
+        <v>57</v>
+      </c>
+      <c r="W84" s="85"/>
+      <c r="X84" s="86"/>
+    </row>
+    <row r="85" spans="4:24" ht="15" customHeight="1">
+      <c r="D85" s="84" t="s">
+        <v>40</v>
+      </c>
+      <c r="E85" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="F85" s="85"/>
+      <c r="G85" s="85"/>
+      <c r="H85" s="85"/>
+      <c r="I85" s="85"/>
+      <c r="J85" s="85"/>
+      <c r="K85" s="85"/>
+      <c r="L85" s="86"/>
+      <c r="N85" s="84" t="s">
+        <v>60</v>
+      </c>
+      <c r="O85" s="85"/>
+      <c r="P85" s="85" t="str">
+        <f ca="1">MID(P83, R85, 1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q85" s="85"/>
+      <c r="R85" s="85">
+        <f ca="1">IF(CLOCK = 1, IF(R85 = (LEN(P83) + 1), 1, R85 + 1),  R85)</f>
+        <v>5</v>
+      </c>
+      <c r="S85" s="85" t="s">
+        <v>61</v>
+      </c>
+      <c r="T85" s="85"/>
+      <c r="U85" s="85"/>
+      <c r="V85" s="85"/>
+      <c r="W85" s="85"/>
+      <c r="X85" s="86"/>
+    </row>
+    <row r="86" spans="4:24" ht="15" customHeight="1">
+      <c r="D86" s="84"/>
+      <c r="E86" s="85"/>
+      <c r="F86" s="85" t="s">
+        <v>4</v>
+      </c>
+      <c r="G86" s="85"/>
+      <c r="H86" s="85"/>
+      <c r="I86" s="85"/>
+      <c r="J86" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="K86" s="85"/>
+      <c r="L86" s="86"/>
+      <c r="N86" s="84"/>
+      <c r="O86" s="85"/>
+      <c r="P86" s="85"/>
+      <c r="Q86" s="85"/>
+      <c r="R86" s="85"/>
+      <c r="S86" s="85"/>
+      <c r="T86" s="85"/>
+      <c r="U86" s="85"/>
+      <c r="V86" s="85"/>
+      <c r="W86" s="85"/>
+      <c r="X86" s="86"/>
+    </row>
+    <row r="87" spans="4:24" ht="15" customHeight="1">
+      <c r="D87" s="84"/>
+      <c r="E87" s="85"/>
+      <c r="F87" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="G87" s="85"/>
+      <c r="H87" s="85"/>
+      <c r="I87" s="85"/>
+      <c r="J87" s="85"/>
+      <c r="K87" s="85"/>
+      <c r="L87" s="86"/>
+      <c r="N87" s="84"/>
+      <c r="O87" s="85"/>
+      <c r="P87" s="85">
+        <v>1</v>
+      </c>
+      <c r="Q87" s="85" t="s">
+        <v>51</v>
+      </c>
+      <c r="R87" s="85"/>
+      <c r="S87" s="85"/>
+      <c r="T87" s="85"/>
+      <c r="U87" s="85"/>
+      <c r="V87" s="85"/>
+      <c r="W87" s="85"/>
+      <c r="X87" s="86"/>
+    </row>
+    <row r="88" spans="4:24" ht="15" customHeight="1">
+      <c r="D88" s="84"/>
+      <c r="E88" s="85"/>
+      <c r="F88" s="85"/>
+      <c r="G88" s="85"/>
+      <c r="H88" s="85" t="s">
+        <v>44</v>
+      </c>
+      <c r="I88" s="85"/>
+      <c r="J88" s="85"/>
+      <c r="K88" s="85"/>
+      <c r="L88" s="86"/>
+      <c r="N88" s="84"/>
+      <c r="O88" s="85"/>
+      <c r="P88" s="85"/>
+      <c r="Q88" s="85"/>
+      <c r="R88" s="85"/>
+      <c r="S88" s="85"/>
+      <c r="T88" s="85"/>
+      <c r="U88" s="85"/>
+      <c r="V88" s="85"/>
+      <c r="W88" s="85"/>
+      <c r="X88" s="86"/>
+    </row>
+    <row r="89" spans="4:24" ht="15" customHeight="1">
+      <c r="D89" s="84"/>
+      <c r="E89" s="85"/>
+      <c r="F89" s="85"/>
+      <c r="G89" s="85"/>
+      <c r="H89" s="85"/>
+      <c r="I89" s="85"/>
+      <c r="J89" s="85"/>
+      <c r="K89" s="85"/>
+      <c r="L89" s="86"/>
+      <c r="N89" s="84"/>
+      <c r="O89" s="85"/>
+      <c r="P89" s="85">
+        <f ca="1">IF(CLOCK = 1, IF(P89 &gt;= P87, 0, P89 + 1), P89)</f>
+        <v>1</v>
+      </c>
+      <c r="Q89" s="85"/>
+      <c r="R89" s="85" t="str">
+        <f ca="1">IF(P89 = P87, IF(LEN(R89) = LEN(P83), "", R89 &amp; P85), R89)</f>
+        <v>1010</v>
+      </c>
+      <c r="S89" s="85"/>
+      <c r="T89" s="85"/>
+      <c r="U89" s="85"/>
+      <c r="V89" s="85"/>
+      <c r="W89" s="85"/>
+      <c r="X89" s="86"/>
+    </row>
+    <row r="90" spans="4:24" ht="15" customHeight="1">
+      <c r="D90" s="84"/>
+      <c r="E90" s="85"/>
+      <c r="F90" s="85"/>
+      <c r="G90" s="85"/>
+      <c r="H90" s="85"/>
+      <c r="I90" s="85"/>
+      <c r="J90" s="85"/>
+      <c r="K90" s="85"/>
+      <c r="L90" s="86"/>
+      <c r="N90" s="87"/>
+      <c r="O90" s="88"/>
+      <c r="P90" s="88" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q90" s="88"/>
+      <c r="R90" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="S90" s="88"/>
+      <c r="T90" s="88"/>
+      <c r="U90" s="88"/>
+      <c r="V90" s="88"/>
+      <c r="W90" s="88"/>
+      <c r="X90" s="89"/>
+    </row>
+    <row r="91" spans="4:24" ht="15" customHeight="1">
+      <c r="D91" s="84"/>
+      <c r="E91" s="85"/>
+      <c r="F91" s="85"/>
+      <c r="G91" s="85"/>
+      <c r="H91" s="85" t="s">
+        <v>48</v>
+      </c>
+      <c r="I91" s="85" t="s">
+        <v>47</v>
+      </c>
+      <c r="J91" s="85"/>
+      <c r="K91" s="85"/>
+      <c r="L91" s="86"/>
+    </row>
+    <row r="92" spans="4:24" ht="15" customHeight="1">
+      <c r="D92" s="84"/>
+      <c r="E92" s="85"/>
+      <c r="F92" s="85"/>
+      <c r="G92" s="85"/>
+      <c r="H92" s="85"/>
+      <c r="I92" s="85"/>
+      <c r="J92" s="85"/>
+      <c r="K92" s="85"/>
+      <c r="L92" s="86"/>
+    </row>
+    <row r="93" spans="4:24" ht="15" customHeight="1">
+      <c r="D93" s="87"/>
+      <c r="E93" s="88"/>
+      <c r="F93" s="88"/>
+      <c r="G93" s="88" t="s">
+        <v>50</v>
+      </c>
+      <c r="H93" s="88" t="s">
+        <v>49</v>
+      </c>
+      <c r="I93" s="88"/>
+      <c r="J93" s="88"/>
+      <c r="K93" s="88"/>
+      <c r="L93" s="89"/>
+    </row>
   </sheetData>
-  <mergeCells count="22">
-    <mergeCell ref="AG50:AG52"/>
-    <mergeCell ref="AG43:AG45"/>
-    <mergeCell ref="AH27:AH29"/>
-    <mergeCell ref="AF35:AF37"/>
-    <mergeCell ref="Y28:Y30"/>
-    <mergeCell ref="W31:W33"/>
-    <mergeCell ref="N36:N38"/>
-    <mergeCell ref="W41:W43"/>
-    <mergeCell ref="N48:N50"/>
-    <mergeCell ref="N24:N26"/>
-    <mergeCell ref="W51:W53"/>
-    <mergeCell ref="W61:W63"/>
-    <mergeCell ref="S71:T71"/>
-    <mergeCell ref="S72:T72"/>
-    <mergeCell ref="N60:N62"/>
+  <mergeCells count="21">
     <mergeCell ref="M5:M7"/>
     <mergeCell ref="X6:X8"/>
     <mergeCell ref="AF8:AF10"/>
@@ -7707,1913 +7909,1847 @@
     <mergeCell ref="N16:N18"/>
     <mergeCell ref="AE18:AE20"/>
     <mergeCell ref="W18:W20"/>
+    <mergeCell ref="W51:W53"/>
+    <mergeCell ref="W61:W63"/>
+    <mergeCell ref="S71:T71"/>
+    <mergeCell ref="S72:T72"/>
+    <mergeCell ref="N60:N62"/>
+    <mergeCell ref="W31:W33"/>
+    <mergeCell ref="N36:N38"/>
+    <mergeCell ref="W41:W43"/>
+    <mergeCell ref="N48:N50"/>
+    <mergeCell ref="N24:N26"/>
+    <mergeCell ref="AG42:AG44"/>
+    <mergeCell ref="AH27:AH29"/>
+    <mergeCell ref="Y28:Y30"/>
+    <mergeCell ref="AG35:AG37"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 V12">
-    <cfRule type="cellIs" dxfId="405" priority="161" operator="equal">
+    <cfRule type="cellIs" dxfId="381" priority="161" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 V12">
-    <cfRule type="cellIs" dxfId="404" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="380" priority="162" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="403" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="379" priority="163" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="402" priority="164" operator="equal">
+    <cfRule type="cellIs" dxfId="378" priority="164" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="401" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="377" priority="165" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="400" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="376" priority="166" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="399" priority="167" operator="equal">
+    <cfRule type="cellIs" dxfId="375" priority="167" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="cellIs" dxfId="398" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="374" priority="168" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="397" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="373" priority="169" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A9">
-    <cfRule type="cellIs" dxfId="396" priority="170" operator="equal">
+    <cfRule type="cellIs" dxfId="372" priority="170" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11 R71">
-    <cfRule type="cellIs" dxfId="395" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="371" priority="171" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11 R71">
-    <cfRule type="cellIs" dxfId="394" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="370" priority="172" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="393" priority="173" operator="equal">
+    <cfRule type="cellIs" dxfId="369" priority="173" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13">
-    <cfRule type="cellIs" dxfId="392" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="368" priority="174" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="391" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="367" priority="175" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
-    <cfRule type="cellIs" dxfId="390" priority="176" operator="equal">
+    <cfRule type="cellIs" dxfId="366" priority="176" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="389" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="365" priority="177" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="388" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="364" priority="178" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="387" priority="179" operator="equal">
+    <cfRule type="cellIs" dxfId="363" priority="179" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A19">
-    <cfRule type="cellIs" dxfId="386" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="362" priority="180" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="385" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="361" priority="181" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="384" priority="182" operator="equal">
+    <cfRule type="cellIs" dxfId="360" priority="182" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="cellIs" dxfId="383" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="359" priority="183" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1">
-    <cfRule type="cellIs" dxfId="382" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="358" priority="184" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="381" priority="185" operator="equal">
+    <cfRule type="cellIs" dxfId="357" priority="185" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="cellIs" dxfId="380" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="356" priority="186" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="379" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="355" priority="187" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="cellIs" dxfId="378" priority="188" operator="equal">
+    <cfRule type="cellIs" dxfId="354" priority="188" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="377" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="353" priority="189" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G12">
-    <cfRule type="cellIs" dxfId="376" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="352" priority="190" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="375" priority="191" operator="equal">
+    <cfRule type="cellIs" dxfId="351" priority="191" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G14">
-    <cfRule type="cellIs" dxfId="374" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="350" priority="192" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T8:U8">
-    <cfRule type="cellIs" dxfId="373" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="349" priority="193" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T8:U8">
-    <cfRule type="cellIs" dxfId="372" priority="194" operator="equal">
+    <cfRule type="cellIs" dxfId="348" priority="194" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="cellIs" dxfId="371" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="347" priority="195" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:V5">
-    <cfRule type="cellIs" dxfId="370" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="346" priority="196" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="369" priority="197" operator="equal">
+    <cfRule type="cellIs" dxfId="345" priority="197" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="368" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="344" priority="198" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="367" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="343" priority="199" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="366" priority="200" operator="equal">
+    <cfRule type="cellIs" dxfId="342" priority="200" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U10">
-    <cfRule type="cellIs" dxfId="365" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="341" priority="201" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U10">
-    <cfRule type="cellIs" dxfId="364" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="340" priority="202" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U12">
-    <cfRule type="cellIs" dxfId="363" priority="203" operator="equal">
+    <cfRule type="cellIs" dxfId="339" priority="203" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U12">
-    <cfRule type="cellIs" dxfId="362" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="338" priority="204" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J5">
-    <cfRule type="cellIs" dxfId="361" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="337" priority="205" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J5">
-    <cfRule type="cellIs" dxfId="360" priority="206" operator="equal">
+    <cfRule type="cellIs" dxfId="336" priority="206" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="359" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="335" priority="207" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="cellIs" dxfId="358" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="334" priority="208" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="357" priority="209" operator="equal">
+    <cfRule type="cellIs" dxfId="333" priority="209" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J9">
-    <cfRule type="cellIs" dxfId="356" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="332" priority="210" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7">
-    <cfRule type="cellIs" dxfId="355" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="331" priority="211" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V7">
-    <cfRule type="cellIs" dxfId="354" priority="212" operator="equal">
+    <cfRule type="cellIs" dxfId="330" priority="212" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V9">
-    <cfRule type="cellIs" dxfId="353" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="329" priority="213" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V9">
-    <cfRule type="cellIs" dxfId="352" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="328" priority="214" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="351" priority="215" operator="equal">
+    <cfRule type="cellIs" dxfId="327" priority="215" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6">
-    <cfRule type="cellIs" dxfId="350" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="326" priority="216" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="349" priority="217" operator="equal">
+    <cfRule type="cellIs" dxfId="325" priority="217" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K8">
-    <cfRule type="cellIs" dxfId="348" priority="218" operator="equal">
+    <cfRule type="cellIs" dxfId="324" priority="218" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="347" priority="219" operator="equal">
+    <cfRule type="cellIs" dxfId="323" priority="219" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12">
-    <cfRule type="cellIs" dxfId="346" priority="220" operator="equal">
+    <cfRule type="cellIs" dxfId="322" priority="220" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="345" priority="221" operator="equal">
+    <cfRule type="cellIs" dxfId="321" priority="221" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14">
-    <cfRule type="cellIs" dxfId="344" priority="222" operator="equal">
+    <cfRule type="cellIs" dxfId="320" priority="222" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" dxfId="343" priority="223" operator="equal">
+    <cfRule type="cellIs" dxfId="319" priority="223" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" dxfId="342" priority="224" operator="equal">
+    <cfRule type="cellIs" dxfId="318" priority="224" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="341" priority="225" operator="equal">
+    <cfRule type="cellIs" dxfId="317" priority="225" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="340" priority="226" operator="equal">
+    <cfRule type="cellIs" dxfId="316" priority="226" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z16">
-    <cfRule type="cellIs" dxfId="339" priority="227" operator="equal">
+    <cfRule type="cellIs" dxfId="315" priority="227" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z16">
-    <cfRule type="cellIs" dxfId="338" priority="228" operator="equal">
+    <cfRule type="cellIs" dxfId="314" priority="228" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB16">
-    <cfRule type="cellIs" dxfId="337" priority="229" operator="equal">
+    <cfRule type="cellIs" dxfId="313" priority="229" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB16">
-    <cfRule type="cellIs" dxfId="336" priority="230" operator="equal">
+    <cfRule type="cellIs" dxfId="312" priority="230" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z19">
-    <cfRule type="cellIs" dxfId="335" priority="231" operator="equal">
+    <cfRule type="cellIs" dxfId="311" priority="231" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z19">
-    <cfRule type="cellIs" dxfId="334" priority="232" operator="equal">
+    <cfRule type="cellIs" dxfId="310" priority="232" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z21">
-    <cfRule type="cellIs" dxfId="333" priority="233" operator="equal">
+    <cfRule type="cellIs" dxfId="309" priority="233" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z21">
-    <cfRule type="cellIs" dxfId="332" priority="234" operator="equal">
+    <cfRule type="cellIs" dxfId="308" priority="234" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23">
-    <cfRule type="cellIs" dxfId="331" priority="235" operator="equal">
+    <cfRule type="cellIs" dxfId="307" priority="235" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z23">
-    <cfRule type="cellIs" dxfId="330" priority="236" operator="equal">
+    <cfRule type="cellIs" dxfId="306" priority="236" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB18">
-    <cfRule type="cellIs" dxfId="329" priority="237" operator="equal">
+    <cfRule type="cellIs" dxfId="305" priority="237" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB18">
-    <cfRule type="cellIs" dxfId="328" priority="238" operator="equal">
+    <cfRule type="cellIs" dxfId="304" priority="238" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB23">
-    <cfRule type="cellIs" dxfId="327" priority="239" operator="equal">
+    <cfRule type="cellIs" dxfId="303" priority="239" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB23">
-    <cfRule type="cellIs" dxfId="326" priority="240" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="240" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="cellIs" dxfId="325" priority="241" operator="equal">
+    <cfRule type="cellIs" dxfId="301" priority="241" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I23">
-    <cfRule type="cellIs" dxfId="324" priority="242" operator="equal">
+    <cfRule type="cellIs" dxfId="300" priority="242" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="323" priority="243" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="243" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K22">
-    <cfRule type="cellIs" dxfId="322" priority="244" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="244" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="321" priority="245" operator="equal">
+    <cfRule type="cellIs" dxfId="297" priority="245" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="320" priority="246" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="246" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26">
-    <cfRule type="cellIs" dxfId="319" priority="247" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="247" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J26">
-    <cfRule type="cellIs" dxfId="318" priority="248" operator="equal">
+    <cfRule type="cellIs" dxfId="294" priority="248" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="cellIs" dxfId="317" priority="249" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="249" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I25">
-    <cfRule type="cellIs" dxfId="316" priority="250" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="250" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="315" priority="251" operator="equal">
+    <cfRule type="cellIs" dxfId="291" priority="251" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H20">
-    <cfRule type="cellIs" dxfId="314" priority="252" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="252" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20">
-    <cfRule type="cellIs" dxfId="313" priority="253" operator="equal">
+    <cfRule type="cellIs" dxfId="289" priority="253" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20">
-    <cfRule type="cellIs" dxfId="312" priority="254" operator="equal">
+    <cfRule type="cellIs" dxfId="288" priority="254" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="311" priority="255" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="255" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="cellIs" dxfId="310" priority="256" operator="equal">
+    <cfRule type="cellIs" dxfId="286" priority="256" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="cellIs" dxfId="309" priority="257" operator="equal">
+    <cfRule type="cellIs" dxfId="285" priority="257" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28">
-    <cfRule type="cellIs" dxfId="308" priority="258" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="258" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="307" priority="259" operator="equal">
+    <cfRule type="cellIs" dxfId="283" priority="259" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L23">
-    <cfRule type="cellIs" dxfId="306" priority="260" operator="equal">
+    <cfRule type="cellIs" dxfId="282" priority="260" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="305" priority="261" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="261" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K30">
-    <cfRule type="cellIs" dxfId="304" priority="262" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="262" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="303" priority="263" operator="equal">
+    <cfRule type="cellIs" dxfId="279" priority="263" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30">
-    <cfRule type="cellIs" dxfId="302" priority="264" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="264" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="301" priority="265" operator="equal">
+    <cfRule type="cellIs" dxfId="277" priority="265" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I35">
-    <cfRule type="cellIs" dxfId="300" priority="266" operator="equal">
+    <cfRule type="cellIs" dxfId="276" priority="266" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="299" priority="267" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="267" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34">
-    <cfRule type="cellIs" dxfId="298" priority="268" operator="equal">
+    <cfRule type="cellIs" dxfId="274" priority="268" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36">
-    <cfRule type="cellIs" dxfId="297" priority="269" operator="equal">
+    <cfRule type="cellIs" dxfId="273" priority="269" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36">
-    <cfRule type="cellIs" dxfId="296" priority="270" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="270" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38">
-    <cfRule type="cellIs" dxfId="295" priority="271" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="271" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J38">
-    <cfRule type="cellIs" dxfId="294" priority="272" operator="equal">
+    <cfRule type="cellIs" dxfId="270" priority="272" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="293" priority="273" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="273" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37">
-    <cfRule type="cellIs" dxfId="292" priority="274" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="274" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="291" priority="275" operator="equal">
+    <cfRule type="cellIs" dxfId="267" priority="275" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="cellIs" dxfId="290" priority="276" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="276" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="289" priority="277" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="277" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J32">
-    <cfRule type="cellIs" dxfId="288" priority="278" operator="equal">
+    <cfRule type="cellIs" dxfId="264" priority="278" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32">
-    <cfRule type="cellIs" dxfId="287" priority="279" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="279" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L32">
-    <cfRule type="cellIs" dxfId="286" priority="280" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="280" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="285" priority="281" operator="equal">
+    <cfRule type="cellIs" dxfId="261" priority="281" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40">
-    <cfRule type="cellIs" dxfId="284" priority="282" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="282" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="cellIs" dxfId="283" priority="283" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="283" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="cellIs" dxfId="282" priority="284" operator="equal">
+    <cfRule type="cellIs" dxfId="258" priority="284" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="281" priority="285" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="285" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42">
-    <cfRule type="cellIs" dxfId="280" priority="286" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="286" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="cellIs" dxfId="279" priority="287" operator="equal">
+    <cfRule type="cellIs" dxfId="255" priority="287" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42">
-    <cfRule type="cellIs" dxfId="278" priority="288" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="288" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="cellIs" dxfId="277" priority="289" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="289" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I47">
-    <cfRule type="cellIs" dxfId="276" priority="290" operator="equal">
+    <cfRule type="cellIs" dxfId="252" priority="290" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46">
-    <cfRule type="cellIs" dxfId="275" priority="291" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="291" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46">
-    <cfRule type="cellIs" dxfId="274" priority="292" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="292" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="cellIs" dxfId="273" priority="293" operator="equal">
+    <cfRule type="cellIs" dxfId="249" priority="293" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48">
-    <cfRule type="cellIs" dxfId="272" priority="294" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="294" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50">
-    <cfRule type="cellIs" dxfId="271" priority="295" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="295" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J50">
-    <cfRule type="cellIs" dxfId="270" priority="296" operator="equal">
+    <cfRule type="cellIs" dxfId="246" priority="296" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="cellIs" dxfId="269" priority="297" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="297" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49">
-    <cfRule type="cellIs" dxfId="268" priority="298" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="298" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="cellIs" dxfId="267" priority="299" operator="equal">
+    <cfRule type="cellIs" dxfId="243" priority="299" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="cellIs" dxfId="266" priority="300" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="300" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44">
-    <cfRule type="cellIs" dxfId="265" priority="301" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="301" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J44">
-    <cfRule type="cellIs" dxfId="264" priority="302" operator="equal">
+    <cfRule type="cellIs" dxfId="240" priority="302" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L44">
-    <cfRule type="cellIs" dxfId="263" priority="303" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="303" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L44">
-    <cfRule type="cellIs" dxfId="262" priority="304" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="304" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52">
-    <cfRule type="cellIs" dxfId="261" priority="305" operator="equal">
+    <cfRule type="cellIs" dxfId="237" priority="305" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I52">
-    <cfRule type="cellIs" dxfId="260" priority="306" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="306" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="259" priority="307" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="307" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="cellIs" dxfId="258" priority="308" operator="equal">
+    <cfRule type="cellIs" dxfId="234" priority="308" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54">
-    <cfRule type="cellIs" dxfId="257" priority="309" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="309" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K54">
-    <cfRule type="cellIs" dxfId="256" priority="310" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="310" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
-    <cfRule type="cellIs" dxfId="255" priority="311" operator="equal">
+    <cfRule type="cellIs" dxfId="231" priority="311" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I54">
-    <cfRule type="cellIs" dxfId="254" priority="312" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="312" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59">
-    <cfRule type="cellIs" dxfId="253" priority="313" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="313" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I59">
-    <cfRule type="cellIs" dxfId="252" priority="314" operator="equal">
+    <cfRule type="cellIs" dxfId="228" priority="314" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="cellIs" dxfId="251" priority="315" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="315" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K58">
-    <cfRule type="cellIs" dxfId="250" priority="316" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="316" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60">
-    <cfRule type="cellIs" dxfId="249" priority="317" operator="equal">
+    <cfRule type="cellIs" dxfId="225" priority="317" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K60">
-    <cfRule type="cellIs" dxfId="248" priority="318" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="318" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J62">
-    <cfRule type="cellIs" dxfId="247" priority="319" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="319" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J62">
-    <cfRule type="cellIs" dxfId="246" priority="320" operator="equal">
+    <cfRule type="cellIs" dxfId="222" priority="320" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61">
-    <cfRule type="cellIs" dxfId="245" priority="321" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="321" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I61">
-    <cfRule type="cellIs" dxfId="244" priority="322" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="322" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="243" priority="323" operator="equal">
+    <cfRule type="cellIs" dxfId="219" priority="323" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H56">
-    <cfRule type="cellIs" dxfId="242" priority="324" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="324" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56">
-    <cfRule type="cellIs" dxfId="241" priority="325" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="325" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56">
-    <cfRule type="cellIs" dxfId="240" priority="326" operator="equal">
+    <cfRule type="cellIs" dxfId="216" priority="326" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="239" priority="327" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="327" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L56">
-    <cfRule type="cellIs" dxfId="238" priority="328" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="328" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64">
-    <cfRule type="cellIs" dxfId="237" priority="329" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="329" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I64">
-    <cfRule type="cellIs" dxfId="236" priority="330" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="330" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59">
-    <cfRule type="cellIs" dxfId="235" priority="331" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="331" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L59">
-    <cfRule type="cellIs" dxfId="234" priority="332" operator="equal">
+    <cfRule type="cellIs" dxfId="210" priority="332" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="cellIs" dxfId="233" priority="333" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="333" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K66">
-    <cfRule type="cellIs" dxfId="232" priority="334" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="334" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66">
-    <cfRule type="cellIs" dxfId="231" priority="335" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="335" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I66">
-    <cfRule type="cellIs" dxfId="230" priority="336" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="336" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K17">
-    <cfRule type="cellIs" dxfId="229" priority="337" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="337" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H16:K17">
-    <cfRule type="cellIs" dxfId="228" priority="338" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="338" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68">
-    <cfRule type="cellIs" dxfId="227" priority="339" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="339" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H68">
-    <cfRule type="cellIs" dxfId="226" priority="340" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="340" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68:M68">
-    <cfRule type="cellIs" dxfId="225" priority="341" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="341" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J68:M68">
-    <cfRule type="cellIs" dxfId="224" priority="342" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="342" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U37">
-    <cfRule type="cellIs" dxfId="223" priority="343" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="343" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U37">
-    <cfRule type="cellIs" dxfId="222" priority="344" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="344" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S33:T33">
-    <cfRule type="cellIs" dxfId="221" priority="345" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="345" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S33:T33">
-    <cfRule type="cellIs" dxfId="220" priority="346" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="346" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S30:U30">
-    <cfRule type="cellIs" dxfId="219" priority="347" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="347" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S30:U30">
-    <cfRule type="cellIs" dxfId="218" priority="348" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="348" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T35">
-    <cfRule type="cellIs" dxfId="217" priority="349" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="349" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T35">
-    <cfRule type="cellIs" dxfId="216" priority="350" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="350" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T37">
-    <cfRule type="cellIs" dxfId="215" priority="351" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="351" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T37">
-    <cfRule type="cellIs" dxfId="214" priority="352" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="352" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U32">
-    <cfRule type="cellIs" dxfId="213" priority="353" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="353" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U32">
-    <cfRule type="cellIs" dxfId="212" priority="354" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="354" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U34">
-    <cfRule type="cellIs" dxfId="211" priority="355" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="355" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U34">
-    <cfRule type="cellIs" dxfId="210" priority="356" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="356" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U47">
-    <cfRule type="cellIs" dxfId="209" priority="357" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="357" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U47">
-    <cfRule type="cellIs" dxfId="208" priority="358" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="358" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S43:T43">
-    <cfRule type="cellIs" dxfId="207" priority="359" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="359" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S43:T43">
-    <cfRule type="cellIs" dxfId="206" priority="360" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="360" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40:U40">
-    <cfRule type="cellIs" dxfId="205" priority="361" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="361" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S40:U40">
-    <cfRule type="cellIs" dxfId="204" priority="362" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="362" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45">
-    <cfRule type="cellIs" dxfId="203" priority="363" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="363" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T45">
-    <cfRule type="cellIs" dxfId="202" priority="364" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="364" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T47">
-    <cfRule type="cellIs" dxfId="201" priority="365" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="365" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T47">
-    <cfRule type="cellIs" dxfId="200" priority="366" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="366" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U42">
-    <cfRule type="cellIs" dxfId="199" priority="367" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="367" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U42">
-    <cfRule type="cellIs" dxfId="198" priority="368" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="368" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U44">
-    <cfRule type="cellIs" dxfId="197" priority="369" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="369" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U44">
-    <cfRule type="cellIs" dxfId="196" priority="370" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="370" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U57">
-    <cfRule type="cellIs" dxfId="195" priority="371" operator="equal">
+    <cfRule type="cellIs" dxfId="171" priority="371" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U57">
-    <cfRule type="cellIs" dxfId="194" priority="372" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="372" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S53:T53">
-    <cfRule type="cellIs" dxfId="193" priority="373" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="373" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S53:T53">
-    <cfRule type="cellIs" dxfId="192" priority="374" operator="equal">
+    <cfRule type="cellIs" dxfId="168" priority="374" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S50:U50">
-    <cfRule type="cellIs" dxfId="191" priority="375" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="375" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S50:U50">
-    <cfRule type="cellIs" dxfId="190" priority="376" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="376" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T55">
-    <cfRule type="cellIs" dxfId="189" priority="377" operator="equal">
+    <cfRule type="cellIs" dxfId="165" priority="377" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T55">
-    <cfRule type="cellIs" dxfId="188" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="378" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T57">
-    <cfRule type="cellIs" dxfId="187" priority="379" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="379" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T57">
-    <cfRule type="cellIs" dxfId="186" priority="380" operator="equal">
+    <cfRule type="cellIs" dxfId="162" priority="380" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U52">
-    <cfRule type="cellIs" dxfId="185" priority="381" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="381" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U52">
-    <cfRule type="cellIs" dxfId="184" priority="382" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="382" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54">
-    <cfRule type="cellIs" dxfId="183" priority="383" operator="equal">
+    <cfRule type="cellIs" dxfId="159" priority="383" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U54">
-    <cfRule type="cellIs" dxfId="182" priority="384" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="384" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U67">
-    <cfRule type="cellIs" dxfId="181" priority="385" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="385" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U67">
-    <cfRule type="cellIs" dxfId="180" priority="386" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="386" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S63:T63">
-    <cfRule type="cellIs" dxfId="179" priority="387" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="387" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S63:T63">
-    <cfRule type="cellIs" dxfId="178" priority="388" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="388" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:U60">
-    <cfRule type="cellIs" dxfId="177" priority="389" operator="equal">
+    <cfRule type="cellIs" dxfId="153" priority="389" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S60:U60">
-    <cfRule type="cellIs" dxfId="176" priority="390" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="390" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T65">
-    <cfRule type="cellIs" dxfId="175" priority="391" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="391" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T65">
-    <cfRule type="cellIs" dxfId="174" priority="392" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="392" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T67">
-    <cfRule type="cellIs" dxfId="173" priority="393" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="393" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T67">
-    <cfRule type="cellIs" dxfId="172" priority="394" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="394" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U62">
-    <cfRule type="cellIs" dxfId="171" priority="395" operator="equal">
+    <cfRule type="cellIs" dxfId="147" priority="395" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U62">
-    <cfRule type="cellIs" dxfId="170" priority="396" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="396" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U64">
-    <cfRule type="cellIs" dxfId="169" priority="397" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="397" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U64">
-    <cfRule type="cellIs" dxfId="168" priority="398" operator="equal">
+    <cfRule type="cellIs" dxfId="144" priority="398" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R25:U26">
-    <cfRule type="cellIs" dxfId="167" priority="399" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="399" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R25:U26">
-    <cfRule type="cellIs" dxfId="166" priority="400" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="400" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W25">
-    <cfRule type="cellIs" dxfId="165" priority="401" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="401" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W25">
-    <cfRule type="cellIs" dxfId="164" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="402" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R71:R72">
-    <cfRule type="cellIs" dxfId="163" priority="403" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="403" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R71:R72">
-    <cfRule type="cellIs" dxfId="162" priority="404" operator="equal">
+    <cfRule type="cellIs" dxfId="138" priority="404" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U72:X72">
-    <cfRule type="cellIs" dxfId="161" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="405" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U72:X72">
-    <cfRule type="cellIs" dxfId="160" priority="406" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="406" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U28">
-    <cfRule type="cellIs" dxfId="159" priority="407" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="407" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U28">
-    <cfRule type="cellIs" dxfId="158" priority="408" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="408" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U38">
-    <cfRule type="cellIs" dxfId="157" priority="409" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="409" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U38">
-    <cfRule type="cellIs" dxfId="156" priority="410" operator="equal">
+    <cfRule type="cellIs" dxfId="132" priority="410" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U48">
-    <cfRule type="cellIs" dxfId="155" priority="411" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="411" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U48">
-    <cfRule type="cellIs" dxfId="154" priority="412" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="412" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U58">
-    <cfRule type="cellIs" dxfId="153" priority="413" operator="equal">
+    <cfRule type="cellIs" dxfId="129" priority="413" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U58">
-    <cfRule type="cellIs" dxfId="152" priority="414" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="414" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7">
-    <cfRule type="cellIs" dxfId="151" priority="415" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="415" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA7">
-    <cfRule type="cellIs" dxfId="150" priority="416" operator="equal">
+    <cfRule type="cellIs" dxfId="126" priority="416" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC6">
-    <cfRule type="cellIs" dxfId="149" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="417" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC6">
-    <cfRule type="cellIs" dxfId="148" priority="418" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="418" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8">
-    <cfRule type="cellIs" dxfId="147" priority="419" operator="equal">
+    <cfRule type="cellIs" dxfId="123" priority="419" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC8">
-    <cfRule type="cellIs" dxfId="146" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="420" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB10">
-    <cfRule type="cellIs" dxfId="145" priority="421" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="421" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB10">
-    <cfRule type="cellIs" dxfId="144" priority="422" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="422" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA9">
-    <cfRule type="cellIs" dxfId="143" priority="423" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="423" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA9">
-    <cfRule type="cellIs" dxfId="142" priority="424" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="424" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z4">
-    <cfRule type="cellIs" dxfId="141" priority="425" operator="equal">
+    <cfRule type="cellIs" dxfId="117" priority="425" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z4">
-    <cfRule type="cellIs" dxfId="140" priority="426" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="426" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4">
-    <cfRule type="cellIs" dxfId="139" priority="427" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="427" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB4">
-    <cfRule type="cellIs" dxfId="138" priority="428" operator="equal">
+    <cfRule type="cellIs" dxfId="114" priority="428" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4">
-    <cfRule type="cellIs" dxfId="137" priority="429" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="429" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD4">
-    <cfRule type="cellIs" dxfId="136" priority="430" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="430" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA12">
-    <cfRule type="cellIs" dxfId="135" priority="431" operator="equal">
+    <cfRule type="cellIs" dxfId="111" priority="431" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA12">
-    <cfRule type="cellIs" dxfId="134" priority="432" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="432" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD7">
-    <cfRule type="cellIs" dxfId="133" priority="433" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="433" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD7">
-    <cfRule type="cellIs" dxfId="132" priority="434" operator="equal">
+    <cfRule type="cellIs" dxfId="108" priority="434" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC14">
-    <cfRule type="cellIs" dxfId="131" priority="435" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="435" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC14">
-    <cfRule type="cellIs" dxfId="130" priority="436" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="436" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA14">
-    <cfRule type="cellIs" dxfId="129" priority="437" operator="equal">
+    <cfRule type="cellIs" dxfId="105" priority="437" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA14">
-    <cfRule type="cellIs" dxfId="128" priority="438" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="438" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23">
-    <cfRule type="cellIs" dxfId="127" priority="439" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="439" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R23">
-    <cfRule type="cellIs" dxfId="126" priority="440" operator="equal">
+    <cfRule type="cellIs" dxfId="102" priority="440" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T23">
-    <cfRule type="cellIs" dxfId="125" priority="441" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="441" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T23">
-    <cfRule type="cellIs" dxfId="124" priority="442" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="442" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20">
-    <cfRule type="cellIs" dxfId="123" priority="443" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="443" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S20">
-    <cfRule type="cellIs" dxfId="122" priority="444" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="444" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T18">
-    <cfRule type="cellIs" dxfId="121" priority="445" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="445" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T18">
-    <cfRule type="cellIs" dxfId="120" priority="446" operator="equal">
+    <cfRule type="cellIs" dxfId="96" priority="446" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB25">
-    <cfRule type="cellIs" dxfId="119" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="159" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB25">
-    <cfRule type="cellIs" dxfId="118" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="160" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD25">
-    <cfRule type="cellIs" dxfId="117" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="93" priority="157" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD25">
-    <cfRule type="cellIs" dxfId="116" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="158" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF25">
-    <cfRule type="cellIs" dxfId="115" priority="155" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="155" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF25">
-    <cfRule type="cellIs" dxfId="114" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="156" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC27">
-    <cfRule type="cellIs" dxfId="113" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="153" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC27">
-    <cfRule type="cellIs" dxfId="112" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="154" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD28">
-    <cfRule type="cellIs" dxfId="111" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="151" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AD28">
-    <cfRule type="cellIs" dxfId="110" priority="152" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="152" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE28">
-    <cfRule type="cellIs" dxfId="109" priority="149" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="149" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE28">
-    <cfRule type="cellIs" dxfId="108" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="150" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC29">
-    <cfRule type="cellIs" dxfId="107" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="147" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC29">
-    <cfRule type="cellIs" dxfId="106" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="148" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC31">
-    <cfRule type="cellIs" dxfId="105" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="145" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC31">
-    <cfRule type="cellIs" dxfId="104" priority="146" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="146" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R16">
-    <cfRule type="cellIs" dxfId="103" priority="143" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="143" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R16">
-    <cfRule type="cellIs" dxfId="102" priority="144" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="144" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16">
-    <cfRule type="cellIs" dxfId="101" priority="141" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="141" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T16">
-    <cfRule type="cellIs" dxfId="100" priority="142" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="142" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD33">
+    <cfRule type="cellIs" dxfId="59" priority="73" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD33">
+    <cfRule type="cellIs" dxfId="58" priority="74" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB34">
-    <cfRule type="cellIs" dxfId="99" priority="139" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="85" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB34">
-    <cfRule type="cellIs" dxfId="98" priority="140" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="86" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC34">
-    <cfRule type="cellIs" dxfId="97" priority="137" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="83" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC34">
-    <cfRule type="cellIs" dxfId="96" priority="138" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="84" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD34">
+    <cfRule type="cellIs" dxfId="53" priority="81" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD34">
+    <cfRule type="cellIs" dxfId="52" priority="82" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE34">
+    <cfRule type="cellIs" dxfId="51" priority="79" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE34">
+    <cfRule type="cellIs" dxfId="50" priority="80" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB33">
+    <cfRule type="cellIs" dxfId="49" priority="77" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB33">
+    <cfRule type="cellIs" dxfId="48" priority="78" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC33">
+    <cfRule type="cellIs" dxfId="47" priority="75" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC33">
+    <cfRule type="cellIs" dxfId="46" priority="76" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD40">
+    <cfRule type="cellIs" dxfId="45" priority="57" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD40">
+    <cfRule type="cellIs" dxfId="44" priority="58" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE33">
+    <cfRule type="cellIs" dxfId="43" priority="71" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE33">
+    <cfRule type="cellIs" dxfId="42" priority="72" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE40">
+    <cfRule type="cellIs" dxfId="41" priority="55" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE40">
+    <cfRule type="cellIs" dxfId="40" priority="56" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB41">
+    <cfRule type="cellIs" dxfId="39" priority="69" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB41">
+    <cfRule type="cellIs" dxfId="38" priority="70" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC41">
+    <cfRule type="cellIs" dxfId="37" priority="67" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC41">
+    <cfRule type="cellIs" dxfId="36" priority="68" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD41">
+    <cfRule type="cellIs" dxfId="35" priority="65" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD41">
+    <cfRule type="cellIs" dxfId="34" priority="66" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE41">
+    <cfRule type="cellIs" dxfId="33" priority="63" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE41">
+    <cfRule type="cellIs" dxfId="32" priority="64" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB40">
+    <cfRule type="cellIs" dxfId="31" priority="61" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB40">
+    <cfRule type="cellIs" dxfId="30" priority="62" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC40">
+    <cfRule type="cellIs" dxfId="29" priority="59" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC40">
+    <cfRule type="cellIs" dxfId="28" priority="60" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE45">
+    <cfRule type="cellIs" dxfId="27" priority="51" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE45">
+    <cfRule type="cellIs" dxfId="26" priority="52" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC45:AD45">
+    <cfRule type="cellIs" dxfId="25" priority="35" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC45:AD45">
+    <cfRule type="cellIs" dxfId="24" priority="36" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB45">
+    <cfRule type="cellIs" dxfId="23" priority="33" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB45">
+    <cfRule type="cellIs" dxfId="22" priority="34" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE43">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE43">
+    <cfRule type="cellIs" dxfId="20" priority="30" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD43">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD43">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB43">
+    <cfRule type="cellIs" dxfId="17" priority="23" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB43">
+    <cfRule type="cellIs" dxfId="16" priority="24" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC43">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC43">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE38">
+    <cfRule type="cellIs" dxfId="13" priority="19" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE38">
+    <cfRule type="cellIs" dxfId="12" priority="20" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC38:AD38">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC38:AD38">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB38">
+    <cfRule type="cellIs" dxfId="9" priority="15" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AB38">
+    <cfRule type="cellIs" dxfId="8" priority="16" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE36">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AE36">
+    <cfRule type="cellIs" dxfId="6" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD36">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AD36">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC36">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC36">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB36">
-    <cfRule type="cellIs" dxfId="95" priority="135" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AB36">
-    <cfRule type="cellIs" dxfId="94" priority="136" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD36">
-    <cfRule type="cellIs" dxfId="93" priority="133" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD36">
-    <cfRule type="cellIs" dxfId="92" priority="134" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD34">
-    <cfRule type="cellIs" dxfId="91" priority="131" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD34">
-    <cfRule type="cellIs" dxfId="90" priority="132" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE34">
-    <cfRule type="cellIs" dxfId="89" priority="129" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE34">
-    <cfRule type="cellIs" dxfId="88" priority="130" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC37">
-    <cfRule type="cellIs" dxfId="87" priority="127" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC37">
-    <cfRule type="cellIs" dxfId="86" priority="128" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC39">
-    <cfRule type="cellIs" dxfId="85" priority="123" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC39">
-    <cfRule type="cellIs" dxfId="84" priority="124" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD41">
-    <cfRule type="cellIs" dxfId="83" priority="73" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD41">
-    <cfRule type="cellIs" dxfId="82" priority="74" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB42">
-    <cfRule type="cellIs" dxfId="81" priority="85" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB42">
-    <cfRule type="cellIs" dxfId="80" priority="86" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC42">
-    <cfRule type="cellIs" dxfId="79" priority="83" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC42">
-    <cfRule type="cellIs" dxfId="78" priority="84" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD42">
-    <cfRule type="cellIs" dxfId="77" priority="81" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD42">
-    <cfRule type="cellIs" dxfId="76" priority="82" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE42">
-    <cfRule type="cellIs" dxfId="75" priority="79" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE42">
-    <cfRule type="cellIs" dxfId="74" priority="80" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB41">
-    <cfRule type="cellIs" dxfId="73" priority="77" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB41">
-    <cfRule type="cellIs" dxfId="72" priority="78" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC41">
-    <cfRule type="cellIs" dxfId="71" priority="75" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC41">
-    <cfRule type="cellIs" dxfId="70" priority="76" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD48">
-    <cfRule type="cellIs" dxfId="69" priority="57" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD48">
-    <cfRule type="cellIs" dxfId="68" priority="58" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE41">
-    <cfRule type="cellIs" dxfId="67" priority="71" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE41">
-    <cfRule type="cellIs" dxfId="66" priority="72" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE48">
-    <cfRule type="cellIs" dxfId="65" priority="55" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE48">
-    <cfRule type="cellIs" dxfId="64" priority="56" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB49">
-    <cfRule type="cellIs" dxfId="63" priority="69" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB49">
-    <cfRule type="cellIs" dxfId="62" priority="70" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC49">
-    <cfRule type="cellIs" dxfId="61" priority="67" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC49">
-    <cfRule type="cellIs" dxfId="60" priority="68" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD49">
-    <cfRule type="cellIs" dxfId="59" priority="65" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD49">
-    <cfRule type="cellIs" dxfId="58" priority="66" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE49">
-    <cfRule type="cellIs" dxfId="57" priority="63" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE49">
-    <cfRule type="cellIs" dxfId="56" priority="64" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB48">
-    <cfRule type="cellIs" dxfId="55" priority="61" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB48">
-    <cfRule type="cellIs" dxfId="54" priority="62" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC48">
-    <cfRule type="cellIs" dxfId="53" priority="59" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC48">
-    <cfRule type="cellIs" dxfId="52" priority="60" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE53">
-    <cfRule type="cellIs" dxfId="49" priority="51" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE53">
-    <cfRule type="cellIs" dxfId="48" priority="52" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC53:AD53">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC53:AD53">
-    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB53">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB53">
-    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE51">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE51">
-    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD51">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD51">
-    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB51">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB51">
-    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC51">
-    <cfRule type="cellIs" dxfId="21" priority="21" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC51">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE46">
-    <cfRule type="cellIs" dxfId="19" priority="19" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE46">
-    <cfRule type="cellIs" dxfId="18" priority="20" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC46:AD46">
-    <cfRule type="cellIs" dxfId="17" priority="17" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC46:AD46">
-    <cfRule type="cellIs" dxfId="16" priority="18" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB46">
-    <cfRule type="cellIs" dxfId="15" priority="15" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB46">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE44">
-    <cfRule type="cellIs" dxfId="13" priority="13" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AE44">
-    <cfRule type="cellIs" dxfId="12" priority="14" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD44">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AD44">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC44">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AC44">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB44">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="AB44">
     <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>

</xml_diff>